<commit_message>
24/03/11 - 01.48AM - Final commit this evening - updated documentation
</commit_message>
<xml_diff>
--- a/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
+++ b/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14600"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="14595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
   <si>
     <t>V11</t>
   </si>
@@ -76,81 +76,6 @@
   </si>
   <si>
     <t>Project folder for code contribution to project</t>
-  </si>
-  <si>
-    <t>I14</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>I15</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>James Nightingale</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1.2_Old</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1.2_Old</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Project folder for code contribution to project</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>V13</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>ppsp-project (project folder)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>James Nightingale, David Russell</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1.1_Current</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Project folder for code contribution to project</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>V14</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>ppsp-davidrussell (project folder</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - various date/time stamps</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>ppsp-jamesnightingale (project folder - various date/time stamps)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -421,12 +346,75 @@
   <si>
     <t>V10</t>
   </si>
+  <si>
+    <r>
+      <t>ppsp-davidrussell (project folder</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - various date/time stamps</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>I14</t>
+  </si>
+  <si>
+    <t>ppsp-jamesnightingale (project folder - various date/time stamps)</t>
+  </si>
+  <si>
+    <t>James Nightingale</t>
+  </si>
+  <si>
+    <t>V13</t>
+  </si>
+  <si>
+    <t>I15</t>
+  </si>
+  <si>
+    <t>ppsp-project (project folder)</t>
+  </si>
+  <si>
+    <t>James Nightingale, David Russell</t>
+  </si>
+  <si>
+    <t>V14</t>
+  </si>
+  <si>
+    <t>Ver_1.5</t>
+  </si>
+  <si>
+    <t>Current Version Project folder</t>
+  </si>
+  <si>
+    <t>Partner Group</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +478,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -536,7 +545,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -566,15 +575,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -587,8 +587,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -621,8 +639,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2108200" y="470534"/>
-          <a:ext cx="218440" cy="261779"/>
+          <a:off x="1847850" y="485774"/>
+          <a:ext cx="218440" cy="277019"/>
           <a:chOff x="1640840" y="238760"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -711,8 +729,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3117215" y="820420"/>
-          <a:ext cx="377825" cy="276860"/>
+          <a:off x="2724150" y="850900"/>
+          <a:ext cx="377825" cy="292100"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -801,8 +819,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3126740" y="1905000"/>
-          <a:ext cx="353060" cy="254794"/>
+          <a:off x="2733675" y="1981200"/>
+          <a:ext cx="353060" cy="262414"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -891,8 +909,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4556124" y="2299334"/>
-          <a:ext cx="742951" cy="236379"/>
+          <a:off x="3990974" y="2390774"/>
+          <a:ext cx="742951" cy="243999"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -981,8 +999,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4660900" y="3406140"/>
-          <a:ext cx="666749" cy="226853"/>
+          <a:off x="4095750" y="3543300"/>
+          <a:ext cx="666749" cy="234473"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1071,8 +1089,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4613275" y="5206364"/>
-          <a:ext cx="742950" cy="245269"/>
+          <a:off x="4048125" y="5419724"/>
+          <a:ext cx="742950" cy="252889"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1161,8 +1179,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7077710" y="5591175"/>
-          <a:ext cx="551180" cy="236379"/>
+          <a:off x="6191250" y="5819775"/>
+          <a:ext cx="551180" cy="243999"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1298,8 +1316,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4527550" y="1183004"/>
-          <a:ext cx="790575" cy="240031"/>
+          <a:off x="3962400" y="1228724"/>
+          <a:ext cx="790575" cy="247651"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1655,108 +1673,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="1"/>
-    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1"/>
+    <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="33.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="73.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="12.5" style="1"/>
+    <col min="7" max="7" width="2.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="73.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="12.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16">
-      <c r="A2" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="A2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>91</v>
+        <v>28</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="23"/>
+      <c r="A3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="20"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="K3" s="8">
         <v>40620</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="18">
-        <v>1.03</v>
+        <v>29</v>
+      </c>
+      <c r="N3" s="30">
+        <v>1.3</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1768,51 +1786,51 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="K4" s="8">
         <v>40620</v>
       </c>
       <c r="L4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="16" t="s">
         <v>32</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="18">
-        <v>1.01</v>
-      </c>
-      <c r="O4" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="6"/>
-      <c r="B5" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="23"/>
+      <c r="B5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="20"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="13" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="K5" s="8">
         <v>40620</v>
@@ -1821,16 +1839,16 @@
         <v>3</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" s="18">
-        <v>1.01</v>
+        <v>31</v>
+      </c>
+      <c r="N5" s="30">
+        <v>1.1000000000000001</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1842,31 +1860,31 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="13" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="K6" s="8">
         <v>40620</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="N6" s="18">
+        <v>46</v>
+      </c>
+      <c r="N6" s="30">
         <v>1</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1874,37 +1892,37 @@
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="13" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="13" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="K7" s="8">
         <v>40620</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" s="18">
+        <v>47</v>
+      </c>
+      <c r="N7" s="30">
         <v>1</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1916,31 +1934,31 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="13" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="K8" s="8">
         <v>40620</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="N8" s="18">
+        <v>60</v>
+      </c>
+      <c r="N8" s="30">
         <v>1</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1948,36 +1966,36 @@
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="E9" s="13" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="13" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="K9" s="8">
         <v>40620</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="N9" s="18">
+        <v>61</v>
+      </c>
+      <c r="N9" s="30">
         <v>1</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1989,69 +2007,69 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="13" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="K10" s="8">
         <v>40620</v>
       </c>
       <c r="L10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="M10" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="N10" s="18">
+      <c r="N10" s="30">
         <v>1</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="6"/>
-      <c r="B11" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="23"/>
+      <c r="B11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="20"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="13" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="K11" s="8">
         <v>40620</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="N11" s="18">
+        <v>63</v>
+      </c>
+      <c r="N11" s="30">
         <v>1</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2063,31 +2081,31 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="13" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="K12" s="8">
         <v>40620</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="N12" s="18">
+        <v>64</v>
+      </c>
+      <c r="N12" s="30">
         <v>1</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2095,37 +2113,37 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="13" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="K13" s="8">
         <v>40621</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="N13" s="18">
-        <v>1.01</v>
+        <v>68</v>
+      </c>
+      <c r="N13" s="30">
+        <v>1.1000000000000001</v>
       </c>
       <c r="O13" s="16" t="s">
         <v>0</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2137,31 +2155,31 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="7" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="K14" s="8">
         <v>40622</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="N14" s="18">
+        <v>72</v>
+      </c>
+      <c r="N14" s="30">
         <v>1</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2170,35 +2188,35 @@
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
       <c r="E15" s="13" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="K15" s="8">
+      <c r="I15" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="25">
         <v>40623</v>
       </c>
-      <c r="L15" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="16" t="s">
+      <c r="L15" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="18">
-        <v>1.01</v>
-      </c>
-      <c r="O15" s="16" t="s">
+      <c r="N15" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="P15" s="9"/>
+      <c r="P15" s="26"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="6"/>
@@ -2208,31 +2226,31 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K16" s="8">
+      <c r="H16" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="25">
         <v>40623</v>
       </c>
-      <c r="L16" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="N16" s="18">
-        <v>1.02</v>
-      </c>
-      <c r="O16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="P16" s="9"/>
+      <c r="L16" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" s="31">
+        <v>1.2</v>
+      </c>
+      <c r="O16" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="P16" s="26"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="6"/>
@@ -2240,35 +2258,35 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="13" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="26" t="s">
+      <c r="H17" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="K17" s="25">
+        <v>40625</v>
+      </c>
+      <c r="L17" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="8">
-        <v>40625</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M17" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="N17" s="18">
-        <v>1.02</v>
-      </c>
-      <c r="O17" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="P17" s="9"/>
+      <c r="M17" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" s="31">
+        <v>1.2</v>
+      </c>
+      <c r="O17" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="P17" s="26"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="6"/>
@@ -2278,14 +2296,30 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="9"/>
+      <c r="H18" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K18" s="8">
+        <v>40626</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="N18" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="O18" s="16" t="s">
+        <v>97</v>
+      </c>
       <c r="P18" s="9"/>
     </row>
     <row r="19" spans="1:16">
@@ -2293,7 +2327,7 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="13" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="6"/>
@@ -2304,7 +2338,7 @@
       <c r="K19" s="7"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
-      <c r="N19" s="18"/>
+      <c r="N19" s="30"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
     </row>
@@ -2322,7 +2356,7 @@
       <c r="K20" s="7"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="18"/>
+      <c r="N20" s="30"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
     </row>
@@ -2332,7 +2366,7 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="13" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="10"/>
@@ -2342,7 +2376,7 @@
       <c r="K21" s="7"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="18"/>
+      <c r="N21" s="30"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
     </row>
@@ -2360,7 +2394,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
-      <c r="N22" s="18"/>
+      <c r="N22" s="30"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
     </row>
@@ -2370,7 +2404,7 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="13" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="10"/>
@@ -2380,7 +2414,7 @@
       <c r="K23" s="7"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
-      <c r="N23" s="18"/>
+      <c r="N23" s="30"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
     </row>
@@ -2398,7 +2432,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
-      <c r="N24" s="18"/>
+      <c r="N24" s="30"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
     </row>
@@ -2408,7 +2442,7 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="13" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="10"/>
@@ -2418,7 +2452,7 @@
       <c r="K25" s="7"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
-      <c r="N25" s="18"/>
+      <c r="N25" s="30"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
     </row>
@@ -2436,7 +2470,7 @@
       <c r="K26" s="7"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
-      <c r="N26" s="18"/>
+      <c r="N26" s="30"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
     </row>
@@ -2445,8 +2479,8 @@
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="22" t="s">
-        <v>83</v>
+      <c r="E27" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -2456,7 +2490,7 @@
       <c r="K27" s="7"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
-      <c r="N27" s="18"/>
+      <c r="N27" s="30"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
     </row>
@@ -2474,7 +2508,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
-      <c r="N28" s="18"/>
+      <c r="N28" s="30"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
     </row>
@@ -2483,7 +2517,7 @@
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -2494,7 +2528,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
-      <c r="N29" s="18"/>
+      <c r="N29" s="30"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
     </row>
@@ -2512,7 +2546,7 @@
       <c r="K30" s="7"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
-      <c r="N30" s="18"/>
+      <c r="N30" s="30"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
     </row>
@@ -2522,7 +2556,7 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="13" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="10"/>
@@ -2532,7 +2566,7 @@
       <c r="K31" s="7"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="18"/>
+      <c r="N31" s="30"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
     </row>
@@ -2550,7 +2584,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
-      <c r="N32" s="18"/>
+      <c r="N32" s="30"/>
       <c r="O32" s="9"/>
       <c r="P32" s="9"/>
     </row>
@@ -2561,7 +2595,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="12" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="12"/>
@@ -2570,7 +2604,7 @@
       <c r="K33" s="12"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
-      <c r="N33" s="18"/>
+      <c r="N33" s="30"/>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
     </row>
@@ -2588,7 +2622,7 @@
       <c r="K34" s="12"/>
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
-      <c r="N34" s="18"/>
+      <c r="N34" s="30"/>
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
     </row>
@@ -2599,7 +2633,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="12" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="12"/>
@@ -2608,7 +2642,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
-      <c r="N35" s="18"/>
+      <c r="N35" s="30"/>
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
     </row>
@@ -2626,7 +2660,7 @@
       <c r="K36" s="12"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
-      <c r="N36" s="18"/>
+      <c r="N36" s="30"/>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
     </row>
@@ -2637,7 +2671,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="12" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="12"/>
@@ -2646,7 +2680,7 @@
       <c r="K37" s="12"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
-      <c r="N37" s="18"/>
+      <c r="N37" s="30"/>
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
     </row>
@@ -2664,7 +2698,7 @@
       <c r="K38" s="12"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
-      <c r="N38" s="18"/>
+      <c r="N38" s="30"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
     </row>
@@ -2674,7 +2708,7 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="13" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="10"/>
@@ -2684,13 +2718,13 @@
       <c r="K39" s="7"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
-      <c r="N39" s="18"/>
+      <c r="N39" s="30"/>
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
     </row>
     <row r="41" spans="1:16">
       <c r="E41" s="16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2706,8 +2740,9 @@
     <hyperlink ref="O2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2717,14 +2752,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -2735,14 +2769,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
25/03/2011 23:50 - Updates from the last few days
</commit_message>
<xml_diff>
--- a/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
+++ b/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="14595"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,245 +55,105 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
-  <si>
-    <t>V11</t>
-  </si>
-  <si>
-    <t>SWVersionControl.xlsx</t>
-  </si>
-  <si>
-    <t>DocVersionControl.xlsx</t>
-  </si>
-  <si>
-    <t>2.2.1_VersionControl</t>
-  </si>
-  <si>
-    <t>I13</t>
-  </si>
-  <si>
-    <t>V12</t>
-  </si>
-  <si>
-    <t>Project folder for code contribution to project</t>
-  </si>
-  <si>
-    <r>
-      <t>Scott Dennison</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, David Russell</t>
-    </r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
+  <si>
+    <t xml:space="preserve">Partner groups revised requirements specification </t>
+  </si>
+  <si>
+    <t>2.3.3_ImplementationDocuments</t>
+  </si>
+  <si>
+    <t>Directory Hierachy</t>
+  </si>
+  <si>
+    <t>I6</t>
+  </si>
+  <si>
+    <t>I8</t>
+  </si>
+  <si>
+    <t>I9</t>
+  </si>
+  <si>
+    <t>I7</t>
+  </si>
+  <si>
+    <t>I10</t>
+  </si>
+  <si>
+    <t>Plan.docx</t>
+  </si>
+  <si>
+    <t>QualityAssurance.docx</t>
+  </si>
+  <si>
+    <t>Requirements.docx</t>
+  </si>
+  <si>
+    <t>ResourceAllocation.docx</t>
+  </si>
+  <si>
+    <t>Strategy.docx</t>
+  </si>
+  <si>
+    <t>Document outlining the plan of the implementation phase</t>
+  </si>
+  <si>
+    <t>Quality assurance document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear and concise requirement specification </t>
+  </si>
+  <si>
+    <t>Document describing the break down of tasks and their allocated resources</t>
+  </si>
+  <si>
+    <t>Document outlining the strategies for the implementation phase</t>
+  </si>
+  <si>
+    <t>David Russell</t>
+  </si>
+  <si>
+    <t>I11</t>
+  </si>
+  <si>
+    <t>CodingStandards.docx</t>
+  </si>
+  <si>
+    <t>Document establish coding standards for all developers</t>
+  </si>
+  <si>
+    <t>2.2.5_CommLogs</t>
+  </si>
+  <si>
+    <t>I12</t>
+  </si>
+  <si>
+    <t>David Russell, Scott Dennison</t>
+  </si>
+  <si>
+    <t>I17</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>Author</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(s)</t>
-    </r>
+    <t>RequirementsTracing.docx</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>staffs-ppsp-repo</t>
-  </si>
-  <si>
-    <t>1_Part1_Specification/Design</t>
-  </si>
-  <si>
-    <t>2_Part2_Implementation</t>
-  </si>
-  <si>
-    <t>2.1_Code</t>
-  </si>
-  <si>
-    <t>2.1.1_Current</t>
-  </si>
-  <si>
-    <t>2.1.2_Old</t>
-  </si>
-  <si>
-    <t>2.2_Control/Logs</t>
-  </si>
-  <si>
-    <t>2.2.2_RepoIndexes</t>
-  </si>
-  <si>
-    <t>2.2.3_Snapshot</t>
-  </si>
-  <si>
-    <t>2.2.4_VersionControl</t>
-  </si>
-  <si>
-    <t>2.3_Documents</t>
-  </si>
-  <si>
-    <t>2.3.1_QualityControl</t>
-  </si>
-  <si>
-    <t>2.3.1.1_Standards</t>
-  </si>
-  <si>
-    <t>2.3.1.2_Testing</t>
-  </si>
-  <si>
-    <t>2.3.1.3_UserSupport</t>
+    <t>David Russell</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>2.3.2_RequirementsTracing</t>
-  </si>
-  <si>
-    <t>Index.xlsx</t>
-  </si>
-  <si>
-    <t>Name of Document</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Index log of all directories and content for the project</t>
-  </si>
-  <si>
-    <t>Index log of all software/operating system versions used for the project</t>
-  </si>
-  <si>
-    <t>Index log of all changes to all directories and content for the project</t>
-  </si>
-  <si>
-    <t>VC3</t>
-  </si>
-  <si>
-    <t>Index ID</t>
-  </si>
-  <si>
-    <t>I1</t>
-  </si>
-  <si>
-    <t>I2</t>
-  </si>
-  <si>
-    <t>I3</t>
-  </si>
-  <si>
-    <t>Current Version</t>
-  </si>
-  <si>
-    <t>VC1, VC2, VC4</t>
-  </si>
-  <si>
-    <t>Date of Creation</t>
-  </si>
-  <si>
-    <t>1.1_BHHSolutions</t>
-  </si>
-  <si>
-    <t>1.1.1_Requirements</t>
-  </si>
-  <si>
-    <t>I4</t>
-  </si>
-  <si>
-    <t>SoftwareRequirements.docx</t>
-  </si>
-  <si>
-    <t>I5</t>
-  </si>
-  <si>
-    <t>SoftwareRequirementsRevised.jpeg</t>
-  </si>
-  <si>
-    <t>Partner group requirements specification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partner groups revised requirements specification </t>
-  </si>
-  <si>
-    <t>2.3.3_ImplementationDocuments</t>
-  </si>
-  <si>
-    <t>Directory Hierachy</t>
-  </si>
-  <si>
-    <t>I6</t>
-  </si>
-  <si>
-    <t>I8</t>
-  </si>
-  <si>
-    <t>I9</t>
-  </si>
-  <si>
-    <t>I7</t>
-  </si>
-  <si>
-    <t>I10</t>
-  </si>
-  <si>
-    <t>Plan.docx</t>
-  </si>
-  <si>
-    <t>QualityAssurance.docx</t>
-  </si>
-  <si>
-    <t>Requirements.docx</t>
-  </si>
-  <si>
-    <t>ResourceAllocation.docx</t>
-  </si>
-  <si>
-    <t>Strategy.docx</t>
-  </si>
-  <si>
-    <t>Document outlining the plan of the implementation phase</t>
-  </si>
-  <si>
-    <t>Quality assurance document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clear and concise requirement specification </t>
-  </si>
-  <si>
-    <t>Document describing the break down of tasks and their allocated resources</t>
-  </si>
-  <si>
-    <t>Document outlining the strategies for the implementation phase</t>
-  </si>
-  <si>
-    <t>David Russell</t>
-  </si>
-  <si>
-    <t>I11</t>
-  </si>
-  <si>
-    <t>CodingStandards.docx</t>
-  </si>
-  <si>
-    <t>Document establish coding standards for all developers</t>
-  </si>
-  <si>
-    <t>2.2.5_CommLogs</t>
-  </si>
-  <si>
-    <t>I12</t>
-  </si>
-  <si>
-    <t>David Russell, Scott Dennison</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Document to map the implemented code to the specified requirements</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>V16</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Document discussing amendments to CodingStandards.docx</t>
@@ -395,9 +255,6 @@
     <t>V14</t>
   </si>
   <si>
-    <t>Ver_1.5</t>
-  </si>
-  <si>
     <t>Current Version Project folder</t>
   </si>
   <si>
@@ -405,6 +262,204 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <r>
+      <t>Ver_1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>I16</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWVersionControl_NEW.xlsx</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scott Dennison</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2.4_VersionControl</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>V15</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>V11</t>
+  </si>
+  <si>
+    <t>SWVersionControl.xlsx</t>
+  </si>
+  <si>
+    <t>DocVersionControl.xlsx</t>
+  </si>
+  <si>
+    <t>2.2.1_VersionControl</t>
+  </si>
+  <si>
+    <t>I13</t>
+  </si>
+  <si>
+    <t>V12</t>
+  </si>
+  <si>
+    <t>Project folder for code contribution to project</t>
+  </si>
+  <si>
+    <r>
+      <t>Scott Dennison</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, David Russell</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Author</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(s)</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>staffs-ppsp-repo</t>
+  </si>
+  <si>
+    <t>1_Part1_Specification/Design</t>
+  </si>
+  <si>
+    <t>2_Part2_Implementation</t>
+  </si>
+  <si>
+    <t>2.1_Code</t>
+  </si>
+  <si>
+    <t>2.1.1_Current</t>
+  </si>
+  <si>
+    <t>2.1.2_Old</t>
+  </si>
+  <si>
+    <t>2.2_Control/Logs</t>
+  </si>
+  <si>
+    <t>2.2.2_RepoIndexes</t>
+  </si>
+  <si>
+    <t>2.2.3_Snapshot</t>
+  </si>
+  <si>
+    <t>2.2.4_VersionControl</t>
+  </si>
+  <si>
+    <t>2.3_Documents</t>
+  </si>
+  <si>
+    <t>2.3.1_QualityControl</t>
+  </si>
+  <si>
+    <t>2.3.1.1_Standards</t>
+  </si>
+  <si>
+    <t>2.3.1.2_Testing</t>
+  </si>
+  <si>
+    <t>2.3.1.3_UserSupport</t>
+  </si>
+  <si>
+    <t>2.3.2_RequirementsTracing</t>
+  </si>
+  <si>
+    <t>Index.xlsx</t>
+  </si>
+  <si>
+    <t>Name of Document</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Index log of all directories and content for the project</t>
+  </si>
+  <si>
+    <t>Index log of all software/operating system versions used for the project</t>
+  </si>
+  <si>
+    <t>Index log of all changes to all directories and content for the project</t>
+  </si>
+  <si>
+    <t>VC3</t>
+  </si>
+  <si>
+    <t>Index ID</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>Current Version</t>
+  </si>
+  <si>
+    <t>VC1, VC2, VC4</t>
+  </si>
+  <si>
+    <t>Date of Creation</t>
+  </si>
+  <si>
+    <t>1.1_BHHSolutions</t>
+  </si>
+  <si>
+    <t>1.1.1_Requirements</t>
+  </si>
+  <si>
+    <t>I4</t>
+  </si>
+  <si>
+    <t>SoftwareRequirements.docx</t>
+  </si>
+  <si>
+    <t>I5</t>
+  </si>
+  <si>
+    <t>SoftwareRequirementsRevised.jpeg</t>
+  </si>
+  <si>
+    <t>Partner group requirements specification</t>
   </si>
 </sst>
 </file>
@@ -414,7 +469,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,6 +554,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -545,7 +613,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -580,13 +648,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -607,6 +668,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -639,8 +714,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1847850" y="485774"/>
-          <a:ext cx="218440" cy="277019"/>
+          <a:off x="2108200" y="460374"/>
+          <a:ext cx="218440" cy="251619"/>
           <a:chOff x="1640840" y="238760"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -729,8 +804,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2724150" y="850900"/>
-          <a:ext cx="377825" cy="292100"/>
+          <a:off x="3114675" y="800100"/>
+          <a:ext cx="377825" cy="266700"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -819,8 +894,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2733675" y="1981200"/>
-          <a:ext cx="353060" cy="262414"/>
+          <a:off x="3124200" y="1854200"/>
+          <a:ext cx="353060" cy="249714"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -909,8 +984,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3990974" y="2390774"/>
-          <a:ext cx="742951" cy="243999"/>
+          <a:off x="4556124" y="2238374"/>
+          <a:ext cx="742951" cy="231299"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -999,8 +1074,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4095750" y="3543300"/>
-          <a:ext cx="666749" cy="234473"/>
+          <a:off x="4660900" y="3314700"/>
+          <a:ext cx="666749" cy="221773"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1089,8 +1164,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4048125" y="5419724"/>
-          <a:ext cx="742950" cy="252889"/>
+          <a:off x="4613275" y="5064124"/>
+          <a:ext cx="742950" cy="240189"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1179,8 +1254,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6191250" y="5819775"/>
-          <a:ext cx="551180" cy="243999"/>
+          <a:off x="7080250" y="5438775"/>
+          <a:ext cx="551180" cy="231299"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1316,8 +1391,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3962400" y="1228724"/>
-          <a:ext cx="790575" cy="247651"/>
+          <a:off x="4527550" y="1152524"/>
+          <a:ext cx="790575" cy="234951"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1673,108 +1748,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A2:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="1"/>
-    <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="1"/>
+    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="61" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="73.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="12.42578125" style="1"/>
+    <col min="10" max="10" width="30.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="73.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5" style="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="12.5" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16">
-      <c r="A2" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="A2" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="18" t="s">
-        <v>78</v>
-      </c>
       <c r="P2" s="17" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="20"/>
+      <c r="A3" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="35"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="K3" s="8">
         <v>40620</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="30">
+        <v>95</v>
+      </c>
+      <c r="N3" s="27">
         <v>1.3</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1785,70 +1860,70 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="K4" s="8">
+      <c r="H4" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="31">
         <v>40620</v>
       </c>
-      <c r="L4" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="30">
+      <c r="L4" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="N4" s="33">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O4" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>32</v>
+      <c r="O4" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="32" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="6"/>
-      <c r="B5" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="20"/>
+      <c r="B5" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="35"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="13" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="K5" s="8">
         <v>40620</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="30">
+        <v>97</v>
+      </c>
+      <c r="N5" s="27">
         <v>1.1000000000000001</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1860,31 +1935,31 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="13" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="K6" s="8">
         <v>40620</v>
       </c>
       <c r="L6" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="N6" s="27">
+        <v>1</v>
+      </c>
+      <c r="O6" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="N6" s="30">
-        <v>1</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="P6" s="16" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1892,37 +1967,37 @@
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="13" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="13" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="K7" s="8">
         <v>40620</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="30">
+        <v>0</v>
+      </c>
+      <c r="N7" s="27">
         <v>1</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1934,31 +2009,31 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="13" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="K8" s="8">
         <v>40620</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="N8" s="30">
+        <v>13</v>
+      </c>
+      <c r="N8" s="27">
         <v>1</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1966,36 +2041,36 @@
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="E9" s="13" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="13" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="K9" s="8">
         <v>40620</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="N9" s="30">
+        <v>14</v>
+      </c>
+      <c r="N9" s="27">
         <v>1</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2007,69 +2082,69 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="K10" s="8">
         <v>40620</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="N10" s="30">
+        <v>15</v>
+      </c>
+      <c r="N10" s="27">
         <v>1</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="6"/>
-      <c r="B11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="20"/>
+      <c r="B11" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="35"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="13" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="K11" s="8">
         <v>40620</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="N11" s="30">
+        <v>16</v>
+      </c>
+      <c r="N11" s="27">
         <v>1</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2081,31 +2156,31 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="13" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="I12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K12" s="8">
         <v>40620</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="N12" s="30">
+        <v>17</v>
+      </c>
+      <c r="N12" s="27">
         <v>1</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2113,37 +2188,37 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="13" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="K13" s="8">
         <v>40621</v>
       </c>
       <c r="L13" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="N13" s="30">
+      <c r="N13" s="27">
         <v>1.1000000000000001</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2155,31 +2230,31 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="7" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="K14" s="8">
         <v>40622</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="N14" s="30">
+        <v>31</v>
+      </c>
+      <c r="N14" s="27">
         <v>1</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2188,35 +2263,35 @@
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
       <c r="E15" s="13" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="K15" s="25">
+      <c r="H15" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="22">
         <v>40623</v>
       </c>
-      <c r="L15" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="31">
+      <c r="L15" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="N15" s="28">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O15" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="P15" s="26"/>
+      <c r="O15" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="P15" s="23"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="6"/>
@@ -2226,31 +2301,31 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="I16" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="K16" s="25">
+      <c r="H16" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="22">
         <v>40623</v>
       </c>
-      <c r="L16" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="M16" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="N16" s="31">
+      <c r="L16" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" s="28">
         <v>1.2</v>
       </c>
-      <c r="O16" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="P16" s="26"/>
+      <c r="O16" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="P16" s="23"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="6"/>
@@ -2258,35 +2333,35 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="13" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="J17" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="K17" s="25">
+      <c r="H17" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" s="22">
         <v>40625</v>
       </c>
-      <c r="L17" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="M17" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="N17" s="31">
+      <c r="L17" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="N17" s="28">
         <v>1.2</v>
       </c>
-      <c r="O17" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="P17" s="26"/>
+      <c r="O17" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="P17" s="23"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="6"/>
@@ -2297,28 +2372,28 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="7" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="K18" s="8">
         <v>40626</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="N18" s="30">
+        <v>57</v>
+      </c>
+      <c r="N18" s="27">
         <v>1.5</v>
       </c>
       <c r="O18" s="16" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="P18" s="9"/>
     </row>
@@ -2327,19 +2402,35 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="13" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="9"/>
+      <c r="H19" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" s="8">
+        <v>40625</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="M19" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="N19" s="27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O19" s="16" t="s">
+        <v>65</v>
+      </c>
       <c r="P19" s="9"/>
     </row>
     <row r="20" spans="1:16">
@@ -2350,14 +2441,30 @@
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="9"/>
+      <c r="H20" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="8">
+        <v>40626</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="N20" s="27">
+        <v>1</v>
+      </c>
+      <c r="O20" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="P20" s="9"/>
     </row>
     <row r="21" spans="1:16">
@@ -2366,7 +2473,7 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="13" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="10"/>
@@ -2376,7 +2483,7 @@
       <c r="K21" s="7"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="30"/>
+      <c r="N21" s="27"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
     </row>
@@ -2394,7 +2501,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
-      <c r="N22" s="30"/>
+      <c r="N22" s="27"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
     </row>
@@ -2404,7 +2511,7 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="13" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="10"/>
@@ -2414,7 +2521,7 @@
       <c r="K23" s="7"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
-      <c r="N23" s="30"/>
+      <c r="N23" s="27"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
     </row>
@@ -2432,7 +2539,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
-      <c r="N24" s="30"/>
+      <c r="N24" s="27"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
     </row>
@@ -2442,7 +2549,7 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="13" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="10"/>
@@ -2452,7 +2559,7 @@
       <c r="K25" s="7"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
-      <c r="N25" s="30"/>
+      <c r="N25" s="27"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
     </row>
@@ -2470,7 +2577,7 @@
       <c r="K26" s="7"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
-      <c r="N26" s="30"/>
+      <c r="N26" s="27"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
     </row>
@@ -2480,7 +2587,7 @@
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="19" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -2490,7 +2597,7 @@
       <c r="K27" s="7"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
-      <c r="N27" s="30"/>
+      <c r="N27" s="27"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
     </row>
@@ -2508,7 +2615,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
-      <c r="N28" s="30"/>
+      <c r="N28" s="27"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
     </row>
@@ -2517,7 +2624,7 @@
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -2528,7 +2635,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
-      <c r="N29" s="30"/>
+      <c r="N29" s="27"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
     </row>
@@ -2546,7 +2653,7 @@
       <c r="K30" s="7"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
-      <c r="N30" s="30"/>
+      <c r="N30" s="27"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
     </row>
@@ -2556,7 +2663,7 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="13" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="10"/>
@@ -2566,7 +2673,7 @@
       <c r="K31" s="7"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="30"/>
+      <c r="N31" s="27"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
     </row>
@@ -2584,7 +2691,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
-      <c r="N32" s="30"/>
+      <c r="N32" s="27"/>
       <c r="O32" s="9"/>
       <c r="P32" s="9"/>
     </row>
@@ -2595,7 +2702,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="12" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="12"/>
@@ -2604,7 +2711,7 @@
       <c r="K33" s="12"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
-      <c r="N33" s="30"/>
+      <c r="N33" s="27"/>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
     </row>
@@ -2622,7 +2729,7 @@
       <c r="K34" s="12"/>
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
-      <c r="N34" s="30"/>
+      <c r="N34" s="27"/>
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
     </row>
@@ -2633,7 +2740,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="12" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="12"/>
@@ -2642,7 +2749,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
-      <c r="N35" s="30"/>
+      <c r="N35" s="27"/>
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
     </row>
@@ -2660,7 +2767,7 @@
       <c r="K36" s="12"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
-      <c r="N36" s="30"/>
+      <c r="N36" s="27"/>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
     </row>
@@ -2671,7 +2778,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="12" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="12"/>
@@ -2680,7 +2787,7 @@
       <c r="K37" s="12"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
-      <c r="N37" s="30"/>
+      <c r="N37" s="27"/>
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
     </row>
@@ -2698,7 +2805,7 @@
       <c r="K38" s="12"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
-      <c r="N38" s="30"/>
+      <c r="N38" s="27"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
     </row>
@@ -2708,7 +2815,7 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="13" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="10"/>
@@ -2718,13 +2825,13 @@
       <c r="K39" s="7"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
-      <c r="N39" s="30"/>
+      <c r="N39" s="27"/>
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
     </row>
     <row r="41" spans="1:16">
       <c r="E41" s="16" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2740,9 +2847,8 @@
     <hyperlink ref="O2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2752,13 +2858,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -2769,13 +2876,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
Signed-off-by: Dave Russell <dave.aj.russell@gmail.com>
</commit_message>
<xml_diff>
--- a/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
+++ b/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14600"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="14595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,171 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
+  <si>
+    <t>V11</t>
+  </si>
+  <si>
+    <t>SWVersionControl.xlsx</t>
+  </si>
+  <si>
+    <t>DocVersionControl.xlsx</t>
+  </si>
+  <si>
+    <t>2.2.1_VersionControl</t>
+  </si>
+  <si>
+    <t>I13</t>
+  </si>
+  <si>
+    <t>V12</t>
+  </si>
+  <si>
+    <t>Project folder for code contribution to project</t>
+  </si>
+  <si>
+    <r>
+      <t>Scott Dennison</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, David Russell</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Author</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(s)</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>staffs-ppsp-repo</t>
+  </si>
+  <si>
+    <t>1_Part1_Specification/Design</t>
+  </si>
+  <si>
+    <t>2_Part2_Implementation</t>
+  </si>
+  <si>
+    <t>2.1_Code</t>
+  </si>
+  <si>
+    <t>2.1.1_Current</t>
+  </si>
+  <si>
+    <t>2.1.2_Old</t>
+  </si>
+  <si>
+    <t>2.2_Control/Logs</t>
+  </si>
+  <si>
+    <t>2.2.2_RepoIndexes</t>
+  </si>
+  <si>
+    <t>2.2.3_Snapshot</t>
+  </si>
+  <si>
+    <t>2.2.4_VersionControl</t>
+  </si>
+  <si>
+    <t>2.3_Documents</t>
+  </si>
+  <si>
+    <t>2.3.1_QualityControl</t>
+  </si>
+  <si>
+    <t>2.3.1.1_Standards</t>
+  </si>
+  <si>
+    <t>2.3.1.2_Testing</t>
+  </si>
+  <si>
+    <t>2.3.1.3_UserSupport</t>
+  </si>
+  <si>
+    <t>2.3.2_RequirementsTracing</t>
+  </si>
+  <si>
+    <t>Index.xlsx</t>
+  </si>
+  <si>
+    <t>Name of Document</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Index log of all directories and content for the project</t>
+  </si>
+  <si>
+    <t>Index log of all software/operating system versions used for the project</t>
+  </si>
+  <si>
+    <t>Index log of all changes to all directories and content for the project</t>
+  </si>
+  <si>
+    <t>VC3</t>
+  </si>
+  <si>
+    <t>Index ID</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>Current Version</t>
+  </si>
+  <si>
+    <t>VC1, VC2, VC4</t>
+  </si>
+  <si>
+    <t>Date of Creation</t>
+  </si>
+  <si>
+    <t>1.1_BHHSolutions</t>
+  </si>
+  <si>
+    <t>1.1.1_Requirements</t>
+  </si>
+  <si>
+    <t>I4</t>
+  </si>
+  <si>
+    <t>SoftwareRequirements.docx</t>
+  </si>
+  <si>
+    <t>I5</t>
+  </si>
+  <si>
+    <t>SoftwareRequirementsRevised.jpeg</t>
+  </si>
+  <si>
+    <t>Partner group requirements specification</t>
+  </si>
   <si>
     <t xml:space="preserve">Partner groups revised requirements specification </t>
   </si>
@@ -130,30 +294,6 @@
   </si>
   <si>
     <t>David Russell, Scott Dennison</t>
-  </si>
-  <si>
-    <t>I17</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>RequirementsTracing.docx</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>David Russell</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.3.2_RequirementsTracing</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Document to map the implemented code to the specified requirements</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>V16</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Document discussing amendments to CodingStandards.docx</t>
@@ -255,6 +395,9 @@
     <t>V14</t>
   </si>
   <si>
+    <t>Ver_1.5</t>
+  </si>
+  <si>
     <t>Current Version Project folder</t>
   </si>
   <si>
@@ -262,204 +405,6 @@
   </si>
   <si>
     <t>Group</t>
-  </si>
-  <si>
-    <r>
-      <t>Ver_1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>I16</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>SWVersionControl_NEW.xlsx</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scott Dennison</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.2.4_VersionControl</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>V15</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>V11</t>
-  </si>
-  <si>
-    <t>SWVersionControl.xlsx</t>
-  </si>
-  <si>
-    <t>DocVersionControl.xlsx</t>
-  </si>
-  <si>
-    <t>2.2.1_VersionControl</t>
-  </si>
-  <si>
-    <t>I13</t>
-  </si>
-  <si>
-    <t>V12</t>
-  </si>
-  <si>
-    <t>Project folder for code contribution to project</t>
-  </si>
-  <si>
-    <r>
-      <t>Scott Dennison</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, David Russell</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Author</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(s)</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>staffs-ppsp-repo</t>
-  </si>
-  <si>
-    <t>1_Part1_Specification/Design</t>
-  </si>
-  <si>
-    <t>2_Part2_Implementation</t>
-  </si>
-  <si>
-    <t>2.1_Code</t>
-  </si>
-  <si>
-    <t>2.1.1_Current</t>
-  </si>
-  <si>
-    <t>2.1.2_Old</t>
-  </si>
-  <si>
-    <t>2.2_Control/Logs</t>
-  </si>
-  <si>
-    <t>2.2.2_RepoIndexes</t>
-  </si>
-  <si>
-    <t>2.2.3_Snapshot</t>
-  </si>
-  <si>
-    <t>2.2.4_VersionControl</t>
-  </si>
-  <si>
-    <t>2.3_Documents</t>
-  </si>
-  <si>
-    <t>2.3.1_QualityControl</t>
-  </si>
-  <si>
-    <t>2.3.1.1_Standards</t>
-  </si>
-  <si>
-    <t>2.3.1.2_Testing</t>
-  </si>
-  <si>
-    <t>2.3.1.3_UserSupport</t>
-  </si>
-  <si>
-    <t>2.3.2_RequirementsTracing</t>
-  </si>
-  <si>
-    <t>Index.xlsx</t>
-  </si>
-  <si>
-    <t>Name of Document</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Index log of all directories and content for the project</t>
-  </si>
-  <si>
-    <t>Index log of all software/operating system versions used for the project</t>
-  </si>
-  <si>
-    <t>Index log of all changes to all directories and content for the project</t>
-  </si>
-  <si>
-    <t>VC3</t>
-  </si>
-  <si>
-    <t>Index ID</t>
-  </si>
-  <si>
-    <t>I1</t>
-  </si>
-  <si>
-    <t>I2</t>
-  </si>
-  <si>
-    <t>I3</t>
-  </si>
-  <si>
-    <t>Current Version</t>
-  </si>
-  <si>
-    <t>VC1, VC2, VC4</t>
-  </si>
-  <si>
-    <t>Date of Creation</t>
-  </si>
-  <si>
-    <t>1.1_BHHSolutions</t>
-  </si>
-  <si>
-    <t>1.1.1_Requirements</t>
-  </si>
-  <si>
-    <t>I4</t>
-  </si>
-  <si>
-    <t>SoftwareRequirements.docx</t>
-  </si>
-  <si>
-    <t>I5</t>
-  </si>
-  <si>
-    <t>SoftwareRequirementsRevised.jpeg</t>
-  </si>
-  <si>
-    <t>Partner group requirements specification</t>
   </si>
 </sst>
 </file>
@@ -469,7 +414,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,19 +499,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -613,7 +545,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -648,6 +580,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -668,20 +607,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -714,8 +639,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2108200" y="460374"/>
-          <a:ext cx="218440" cy="251619"/>
+          <a:off x="1847850" y="485774"/>
+          <a:ext cx="218440" cy="277019"/>
           <a:chOff x="1640840" y="238760"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -804,8 +729,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3114675" y="800100"/>
-          <a:ext cx="377825" cy="266700"/>
+          <a:off x="2724150" y="850900"/>
+          <a:ext cx="377825" cy="292100"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -894,8 +819,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3124200" y="1854200"/>
-          <a:ext cx="353060" cy="249714"/>
+          <a:off x="2733675" y="1981200"/>
+          <a:ext cx="353060" cy="262414"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -984,8 +909,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4556124" y="2238374"/>
-          <a:ext cx="742951" cy="231299"/>
+          <a:off x="3990974" y="2390774"/>
+          <a:ext cx="742951" cy="243999"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1074,8 +999,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4660900" y="3314700"/>
-          <a:ext cx="666749" cy="221773"/>
+          <a:off x="4095750" y="3543300"/>
+          <a:ext cx="666749" cy="234473"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1164,8 +1089,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4613275" y="5064124"/>
-          <a:ext cx="742950" cy="240189"/>
+          <a:off x="4048125" y="5419724"/>
+          <a:ext cx="742950" cy="252889"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1254,8 +1179,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7080250" y="5438775"/>
-          <a:ext cx="551180" cy="231299"/>
+          <a:off x="6191250" y="5819775"/>
+          <a:ext cx="551180" cy="243999"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1391,8 +1316,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4527550" y="1152524"/>
-          <a:ext cx="790575" cy="234951"/>
+          <a:off x="3962400" y="1228724"/>
+          <a:ext cx="790575" cy="247651"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1748,108 +1673,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="1"/>
-    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1"/>
+    <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="61" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="33.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="73.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="12.5" style="1"/>
+    <col min="10" max="10" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="73.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="12.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16">
-      <c r="A2" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="A2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>103</v>
+        <v>28</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="35"/>
+      <c r="A3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="20"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="K3" s="8">
         <v>40620</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="N3" s="27">
+        <v>29</v>
+      </c>
+      <c r="N3" s="30">
         <v>1.3</v>
       </c>
       <c r="O3" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>38</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1860,70 +1785,70 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" s="24" t="s">
+      <c r="H4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="8">
+        <v>40620</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="31">
-        <v>40620</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="M4" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="N4" s="33">
+      <c r="M4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="30">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="32" t="s">
-        <v>98</v>
+      <c r="O4" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="6"/>
-      <c r="B5" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="35"/>
+      <c r="B5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="20"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="13" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="K5" s="8">
         <v>40620</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="N5" s="27">
+        <v>31</v>
+      </c>
+      <c r="N5" s="30">
         <v>1.1000000000000001</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>98</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1935,31 +1860,31 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="13" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="K6" s="8">
         <v>40620</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="N6" s="27">
+        <v>46</v>
+      </c>
+      <c r="N6" s="30">
         <v>1</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1967,37 +1892,37 @@
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="13" t="s">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="13" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>111</v>
+        <v>45</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="K7" s="8">
         <v>40620</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="N7" s="27">
+        <v>47</v>
+      </c>
+      <c r="N7" s="30">
         <v>1</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -2009,31 +1934,31 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="13" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="K8" s="8">
         <v>40620</v>
       </c>
       <c r="L8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" s="30">
         <v>1</v>
       </c>
-      <c r="M8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="27">
-        <v>1</v>
-      </c>
       <c r="O8" s="16" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -2041,36 +1966,36 @@
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="E9" s="13" t="s">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="13" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="K9" s="8">
         <v>40620</v>
       </c>
       <c r="L9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" s="30">
         <v>1</v>
       </c>
-      <c r="M9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="27">
-        <v>1</v>
-      </c>
       <c r="O9" s="16" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2082,69 +2007,69 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="13" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="K10" s="8">
         <v>40620</v>
       </c>
       <c r="L10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="N10" s="30">
         <v>1</v>
       </c>
-      <c r="M10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="27">
-        <v>1</v>
-      </c>
       <c r="O10" s="16" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="6"/>
-      <c r="B11" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="35"/>
+      <c r="B11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="20"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="13" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="K11" s="8">
         <v>40620</v>
       </c>
       <c r="L11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="N11" s="30">
         <v>1</v>
       </c>
-      <c r="M11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="27">
-        <v>1</v>
-      </c>
       <c r="O11" s="16" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2156,31 +2081,31 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="13" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="K12" s="8">
         <v>40620</v>
       </c>
       <c r="L12" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="N12" s="30">
         <v>1</v>
       </c>
-      <c r="M12" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="N12" s="27">
-        <v>1</v>
-      </c>
       <c r="O12" s="16" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2188,37 +2113,37 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="13" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="K13" s="8">
         <v>40621</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="27">
+        <v>68</v>
+      </c>
+      <c r="N13" s="30">
         <v>1.1000000000000001</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2230,31 +2155,31 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="7" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="K14" s="8">
         <v>40622</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="N14" s="27">
+        <v>72</v>
+      </c>
+      <c r="N14" s="30">
         <v>1</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2263,35 +2188,35 @@
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
       <c r="E15" s="13" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="22">
+      <c r="H15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="25">
         <v>40623</v>
       </c>
-      <c r="L15" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="M15" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N15" s="28">
+      <c r="L15" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="31">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O15" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="P15" s="23"/>
+      <c r="O15" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" s="26"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="6"/>
@@ -2301,31 +2226,31 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="K16" s="22">
+      <c r="H16" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="25">
         <v>40623</v>
       </c>
-      <c r="L16" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="M16" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N16" s="28">
+      <c r="L16" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" s="31">
         <v>1.2</v>
       </c>
-      <c r="O16" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="P16" s="23"/>
+      <c r="O16" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="P16" s="26"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="6"/>
@@ -2333,35 +2258,35 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="13" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="K17" s="22">
+      <c r="H17" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="K17" s="25">
         <v>40625</v>
       </c>
-      <c r="L17" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="M17" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N17" s="28">
+      <c r="L17" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" s="31">
         <v>1.2</v>
       </c>
-      <c r="O17" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="P17" s="23"/>
+      <c r="O17" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="P17" s="26"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="6"/>
@@ -2372,28 +2297,28 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="7" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="K18" s="8">
         <v>40626</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="N18" s="27">
+        <v>99</v>
+      </c>
+      <c r="N18" s="30">
         <v>1.5</v>
       </c>
       <c r="O18" s="16" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="P18" s="9"/>
     </row>
@@ -2402,35 +2327,19 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="13" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="K19" s="8">
-        <v>40625</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="M19" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="N19" s="27">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="O19" s="16" t="s">
-        <v>65</v>
-      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="9"/>
       <c r="P19" s="9"/>
     </row>
     <row r="20" spans="1:16">
@@ -2441,30 +2350,14 @@
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="K20" s="8">
-        <v>40626</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="N20" s="27">
-        <v>1</v>
-      </c>
-      <c r="O20" s="16" t="s">
-        <v>30</v>
-      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="9"/>
       <c r="P20" s="9"/>
     </row>
     <row r="21" spans="1:16">
@@ -2473,7 +2366,7 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="13" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="10"/>
@@ -2483,7 +2376,7 @@
       <c r="K21" s="7"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="27"/>
+      <c r="N21" s="30"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
     </row>
@@ -2501,7 +2394,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
-      <c r="N22" s="27"/>
+      <c r="N22" s="30"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
     </row>
@@ -2511,7 +2404,7 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="13" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="10"/>
@@ -2521,7 +2414,7 @@
       <c r="K23" s="7"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
-      <c r="N23" s="27"/>
+      <c r="N23" s="30"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
     </row>
@@ -2539,7 +2432,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
-      <c r="N24" s="27"/>
+      <c r="N24" s="30"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
     </row>
@@ -2549,7 +2442,7 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="13" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="10"/>
@@ -2559,7 +2452,7 @@
       <c r="K25" s="7"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
-      <c r="N25" s="27"/>
+      <c r="N25" s="30"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
     </row>
@@ -2577,7 +2470,7 @@
       <c r="K26" s="7"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
-      <c r="N26" s="27"/>
+      <c r="N26" s="30"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
     </row>
@@ -2587,7 +2480,7 @@
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="19" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -2597,7 +2490,7 @@
       <c r="K27" s="7"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
-      <c r="N27" s="27"/>
+      <c r="N27" s="30"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
     </row>
@@ -2615,7 +2508,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
-      <c r="N28" s="27"/>
+      <c r="N28" s="30"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
     </row>
@@ -2624,7 +2517,7 @@
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -2635,7 +2528,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
-      <c r="N29" s="27"/>
+      <c r="N29" s="30"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
     </row>
@@ -2653,7 +2546,7 @@
       <c r="K30" s="7"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
-      <c r="N30" s="27"/>
+      <c r="N30" s="30"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
     </row>
@@ -2663,7 +2556,7 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="13" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="10"/>
@@ -2673,7 +2566,7 @@
       <c r="K31" s="7"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="27"/>
+      <c r="N31" s="30"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
     </row>
@@ -2691,7 +2584,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
-      <c r="N32" s="27"/>
+      <c r="N32" s="30"/>
       <c r="O32" s="9"/>
       <c r="P32" s="9"/>
     </row>
@@ -2702,7 +2595,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="12" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="12"/>
@@ -2711,7 +2604,7 @@
       <c r="K33" s="12"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
-      <c r="N33" s="27"/>
+      <c r="N33" s="30"/>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
     </row>
@@ -2729,7 +2622,7 @@
       <c r="K34" s="12"/>
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
-      <c r="N34" s="27"/>
+      <c r="N34" s="30"/>
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
     </row>
@@ -2740,7 +2633,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="12" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="12"/>
@@ -2749,7 +2642,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
-      <c r="N35" s="27"/>
+      <c r="N35" s="30"/>
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
     </row>
@@ -2767,7 +2660,7 @@
       <c r="K36" s="12"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
-      <c r="N36" s="27"/>
+      <c r="N36" s="30"/>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
     </row>
@@ -2778,7 +2671,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="12" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="12"/>
@@ -2787,7 +2680,7 @@
       <c r="K37" s="12"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
-      <c r="N37" s="27"/>
+      <c r="N37" s="30"/>
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
     </row>
@@ -2805,7 +2698,7 @@
       <c r="K38" s="12"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
-      <c r="N38" s="27"/>
+      <c r="N38" s="30"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
     </row>
@@ -2815,7 +2708,7 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="13" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="10"/>
@@ -2825,13 +2718,13 @@
       <c r="K39" s="7"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
-      <c r="N39" s="27"/>
+      <c r="N39" s="30"/>
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
     </row>
     <row r="41" spans="1:16">
       <c r="E41" s="16" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2847,8 +2740,9 @@
     <hyperlink ref="O2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2858,14 +2752,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -2876,14 +2769,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
28/03/2011 - 20.09 commit of today's work Signed-off-by: Dave Russell <dave.aj.russell@gmail.com>
</commit_message>
<xml_diff>
--- a/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
+++ b/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
@@ -24,6 +24,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Dave</author>
+    <author>David Russell</author>
   </authors>
   <commentList>
     <comment ref="O14" authorId="0">
@@ -46,7 +47,31 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Unlikely to change - not change control required</t>
+Will not change - not change control required</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O21" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Russell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Again, this doucment will not change</t>
         </r>
       </text>
     </comment>
@@ -55,7 +80,211 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="138">
+  <si>
+    <t>Visio drawing containing some new designs which were not included in BHH document, which are required for our implementation</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnnotatedRequirements.docx</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scott Dennison</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Requirements with some annotations which we must design for</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestCases.docx</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1_Part1_Specification/Design</t>
+  </si>
+  <si>
+    <t>2_Part2_Implementation</t>
+  </si>
+  <si>
+    <t>2.1_Code</t>
+  </si>
+  <si>
+    <t>2.1.1_Current</t>
+  </si>
+  <si>
+    <t>2.1.2_Old</t>
+  </si>
+  <si>
+    <t>2.2_Control/Logs</t>
+  </si>
+  <si>
+    <t>2.2.2_RepoIndexes</t>
+  </si>
+  <si>
+    <t>2.2.3_Snapshot</t>
+  </si>
+  <si>
+    <t>2.2.4_VersionControl</t>
+  </si>
+  <si>
+    <t>2.3_Documents</t>
+  </si>
+  <si>
+    <t>2.3.1_QualityControl</t>
+  </si>
+  <si>
+    <t>2.3.1.1_Standards</t>
+  </si>
+  <si>
+    <t>2.3.1.2_Testing</t>
+  </si>
+  <si>
+    <t>2.3.1.3_UserSupport</t>
+  </si>
+  <si>
+    <t>2.3.2_RequirementsTracing</t>
+  </si>
+  <si>
+    <t>Index.xlsx</t>
+  </si>
+  <si>
+    <t>Name of Document</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Index log of all directories and content for the project</t>
+  </si>
+  <si>
+    <t>Index log of all software/operating system versions used for the project</t>
+  </si>
+  <si>
+    <t>Index log of all changes to all directories and content for the project</t>
+  </si>
+  <si>
+    <t>VC3</t>
+  </si>
+  <si>
+    <t>Index ID</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>Current Version</t>
+  </si>
+  <si>
+    <t>VC1, VC2, VC4</t>
+  </si>
+  <si>
+    <t>Date of Creation</t>
+  </si>
+  <si>
+    <t>1.1_BHHSolutions</t>
+  </si>
+  <si>
+    <t>1.1.1_Requirements</t>
+  </si>
+  <si>
+    <t>I4</t>
+  </si>
+  <si>
+    <t>SoftwareRequirements.docx</t>
+  </si>
+  <si>
+    <t>I5</t>
+  </si>
+  <si>
+    <t>SoftwareRequirementsRevised.jpeg</t>
+  </si>
+  <si>
+    <t>Partner group requirements specification</t>
+  </si>
+  <si>
+    <t>I18</t>
+  </si>
+  <si>
+    <t>I19</t>
+  </si>
+  <si>
+    <t>I20</t>
+  </si>
+  <si>
+    <t>I21</t>
+  </si>
+  <si>
+    <t>I22</t>
+  </si>
+  <si>
+    <t>V19</t>
+  </si>
+  <si>
+    <t>V20</t>
+  </si>
+  <si>
+    <t>DesignReview.docx</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>David Russell</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3.3_ImplementationDocuments</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Digital write up copy of the minutes for the design review meeting with BHH</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>BasisPathTesting.docx</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>David Russell, James Nightingale</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>James Nightingale</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Document containing the basis path testing flow diagrams</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>V17</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Document containing the test cases</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>V18</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>NewDesigns.vsd</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
   <si>
     <t xml:space="preserve">Partner groups revised requirements specification </t>
   </si>
@@ -350,117 +579,6 @@
   <si>
     <t>staffs-ppsp-repo</t>
   </si>
-  <si>
-    <t>1_Part1_Specification/Design</t>
-  </si>
-  <si>
-    <t>2_Part2_Implementation</t>
-  </si>
-  <si>
-    <t>2.1_Code</t>
-  </si>
-  <si>
-    <t>2.1.1_Current</t>
-  </si>
-  <si>
-    <t>2.1.2_Old</t>
-  </si>
-  <si>
-    <t>2.2_Control/Logs</t>
-  </si>
-  <si>
-    <t>2.2.2_RepoIndexes</t>
-  </si>
-  <si>
-    <t>2.2.3_Snapshot</t>
-  </si>
-  <si>
-    <t>2.2.4_VersionControl</t>
-  </si>
-  <si>
-    <t>2.3_Documents</t>
-  </si>
-  <si>
-    <t>2.3.1_QualityControl</t>
-  </si>
-  <si>
-    <t>2.3.1.1_Standards</t>
-  </si>
-  <si>
-    <t>2.3.1.2_Testing</t>
-  </si>
-  <si>
-    <t>2.3.1.3_UserSupport</t>
-  </si>
-  <si>
-    <t>2.3.2_RequirementsTracing</t>
-  </si>
-  <si>
-    <t>Index.xlsx</t>
-  </si>
-  <si>
-    <t>Name of Document</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Index log of all directories and content for the project</t>
-  </si>
-  <si>
-    <t>Index log of all software/operating system versions used for the project</t>
-  </si>
-  <si>
-    <t>Index log of all changes to all directories and content for the project</t>
-  </si>
-  <si>
-    <t>VC3</t>
-  </si>
-  <si>
-    <t>Index ID</t>
-  </si>
-  <si>
-    <t>I1</t>
-  </si>
-  <si>
-    <t>I2</t>
-  </si>
-  <si>
-    <t>I3</t>
-  </si>
-  <si>
-    <t>Current Version</t>
-  </si>
-  <si>
-    <t>VC1, VC2, VC4</t>
-  </si>
-  <si>
-    <t>Date of Creation</t>
-  </si>
-  <si>
-    <t>1.1_BHHSolutions</t>
-  </si>
-  <si>
-    <t>1.1.1_Requirements</t>
-  </si>
-  <si>
-    <t>I4</t>
-  </si>
-  <si>
-    <t>SoftwareRequirements.docx</t>
-  </si>
-  <si>
-    <t>I5</t>
-  </si>
-  <si>
-    <t>SoftwareRequirementsRevised.jpeg</t>
-  </si>
-  <si>
-    <t>Partner group requirements specification</t>
-  </si>
 </sst>
 </file>
 
@@ -469,7 +587,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,6 +685,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -643,7 +774,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -682,6 +812,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -714,8 +847,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2108200" y="460374"/>
-          <a:ext cx="218440" cy="251619"/>
+          <a:off x="2108200" y="477307"/>
+          <a:ext cx="218440" cy="268553"/>
           <a:chOff x="1640840" y="238760"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -804,8 +937,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3114675" y="800100"/>
-          <a:ext cx="377825" cy="266700"/>
+          <a:off x="3110442" y="833967"/>
+          <a:ext cx="377825" cy="283633"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -894,8 +1027,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3124200" y="1854200"/>
-          <a:ext cx="353060" cy="249714"/>
+          <a:off x="3119967" y="1938867"/>
+          <a:ext cx="353060" cy="258180"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -984,8 +1117,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4556124" y="2238374"/>
-          <a:ext cx="742951" cy="231299"/>
+          <a:off x="4556124" y="2339974"/>
+          <a:ext cx="742951" cy="239766"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1074,8 +1207,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4660900" y="3314700"/>
-          <a:ext cx="666749" cy="221773"/>
+          <a:off x="4660900" y="3467100"/>
+          <a:ext cx="666749" cy="230240"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1164,8 +1297,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4613275" y="5064124"/>
-          <a:ext cx="742950" cy="240189"/>
+          <a:off x="4613275" y="5470524"/>
+          <a:ext cx="742950" cy="248656"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1254,8 +1387,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7080250" y="5438775"/>
-          <a:ext cx="551180" cy="231299"/>
+          <a:off x="7084483" y="5862108"/>
+          <a:ext cx="551180" cy="239766"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1391,8 +1524,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4527550" y="1152524"/>
-          <a:ext cx="790575" cy="234951"/>
+          <a:off x="4527550" y="1203324"/>
+          <a:ext cx="790575" cy="243418"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1751,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A2:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="14"/>
@@ -1770,86 +1903,86 @@
     <col min="11" max="11" width="20.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="33.5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="73.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5" style="28" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="12.5" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16">
-      <c r="A2" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="A2" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>37</v>
-      </c>
       <c r="P2" s="17" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="35"/>
+      <c r="A3" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="34"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="K3" s="8">
         <v>40620</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="N3" s="27">
+        <v>24</v>
+      </c>
+      <c r="N3" s="26">
         <v>1.3</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1860,70 +1993,70 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="30">
+        <v>40620</v>
+      </c>
+      <c r="L4" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O4" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="31">
-        <v>40620</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="M4" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="N4" s="33">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="O4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="32" t="s">
-        <v>98</v>
+      <c r="P4" s="31" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="6"/>
-      <c r="B5" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="35"/>
+      <c r="B5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="13" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="K5" s="8">
         <v>40620</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="N5" s="27">
+        <v>26</v>
+      </c>
+      <c r="N5" s="26">
         <v>1.1000000000000001</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>98</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1935,31 +2068,31 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="13" t="s">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="K6" s="8">
         <v>40620</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>107</v>
+        <v>36</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="N6" s="27">
+        <v>41</v>
+      </c>
+      <c r="N6" s="26">
         <v>1</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1967,37 +2100,37 @@
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="13" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="13" t="s">
-        <v>110</v>
+        <v>39</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="K7" s="8">
         <v>40620</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>107</v>
+        <v>36</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="N7" s="27">
+        <v>62</v>
+      </c>
+      <c r="N7" s="26">
         <v>1</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -2009,31 +2142,31 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="13" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="K8" s="8">
         <v>40620</v>
       </c>
       <c r="L8" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="26">
         <v>1</v>
       </c>
-      <c r="M8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="27">
-        <v>1</v>
-      </c>
       <c r="O8" s="16" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -2041,36 +2174,36 @@
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="E9" s="13" t="s">
-        <v>107</v>
+        <v>36</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="13" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="K9" s="8">
         <v>40620</v>
       </c>
       <c r="L9" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" s="26">
         <v>1</v>
       </c>
-      <c r="M9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="27">
-        <v>1</v>
-      </c>
       <c r="O9" s="16" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2082,69 +2215,69 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="13" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="K10" s="8">
         <v>40620</v>
       </c>
       <c r="L10" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="N10" s="26">
         <v>1</v>
       </c>
-      <c r="M10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="27">
-        <v>1</v>
-      </c>
       <c r="O10" s="16" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="6"/>
-      <c r="B11" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="35"/>
+      <c r="B11" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="34"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="13" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="K11" s="8">
         <v>40620</v>
       </c>
       <c r="L11" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" s="26">
         <v>1</v>
       </c>
-      <c r="M11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="27">
-        <v>1</v>
-      </c>
       <c r="O11" s="16" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2156,31 +2289,31 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="13" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="K12" s="8">
         <v>40620</v>
       </c>
       <c r="L12" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="N12" s="26">
         <v>1</v>
       </c>
-      <c r="M12" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="N12" s="27">
-        <v>1</v>
-      </c>
       <c r="O12" s="16" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2188,37 +2321,37 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="13" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="K13" s="8">
         <v>40621</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="27">
+        <v>83</v>
+      </c>
+      <c r="N13" s="26">
         <v>1.1000000000000001</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2230,31 +2363,31 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="7" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="K14" s="8">
         <v>40622</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="N14" s="27">
+        <v>93</v>
+      </c>
+      <c r="N14" s="26">
         <v>1</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2263,35 +2396,35 @@
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
       <c r="E15" s="13" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="22">
+      <c r="H15" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" s="21">
         <v>40623</v>
       </c>
-      <c r="L15" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="M15" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N15" s="28">
+      <c r="L15" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="N15" s="27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O15" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="P15" s="23"/>
+      <c r="O15" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="P15" s="22"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="6"/>
@@ -2301,31 +2434,31 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="K16" s="22">
+      <c r="H16" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="K16" s="21">
         <v>40623</v>
       </c>
-      <c r="L16" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="M16" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N16" s="28">
+      <c r="L16" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16" s="27">
         <v>1.2</v>
       </c>
-      <c r="O16" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="P16" s="23"/>
+      <c r="O16" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="P16" s="22"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="6"/>
@@ -2333,35 +2466,35 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="13" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="K17" s="22">
+      <c r="H17" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="K17" s="21">
         <v>40625</v>
       </c>
-      <c r="L17" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="M17" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N17" s="28">
+      <c r="L17" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="N17" s="27">
         <v>1.2</v>
       </c>
-      <c r="O17" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="P17" s="23"/>
+      <c r="O17" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="P17" s="22"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="6"/>
@@ -2372,28 +2505,28 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="7" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="K18" s="8">
         <v>40626</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="N18" s="27">
-        <v>1.5</v>
+        <v>119</v>
+      </c>
+      <c r="N18" s="26">
+        <v>1.6</v>
       </c>
       <c r="O18" s="16" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="P18" s="9"/>
     </row>
@@ -2402,34 +2535,34 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="13" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>63</v>
+      <c r="H19" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="J19" s="29" t="s">
+        <v>125</v>
       </c>
       <c r="K19" s="8">
         <v>40625</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="M19" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="N19" s="27">
+        <v>126</v>
+      </c>
+      <c r="M19" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" s="26">
         <v>1.1000000000000001</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="P19" s="9"/>
     </row>
@@ -2441,29 +2574,29 @@
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="30" t="s">
-        <v>27</v>
+      <c r="H20" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>89</v>
       </c>
       <c r="K20" s="8">
         <v>40626</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="N20" s="27">
+        <v>91</v>
+      </c>
+      <c r="N20" s="26">
         <v>1</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="P20" s="9"/>
     </row>
@@ -2473,18 +2606,34 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="13" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="9"/>
+      <c r="H21" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" s="8">
+        <v>40630</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="26">
+        <v>1</v>
+      </c>
+      <c r="O21" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="P21" s="9"/>
     </row>
     <row r="22" spans="1:16">
@@ -2495,14 +2644,30 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="9"/>
+      <c r="H22" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" s="8">
+        <v>40629</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="N22" s="26">
+        <v>1</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="P22" s="9"/>
     </row>
     <row r="23" spans="1:16">
@@ -2511,21 +2676,37 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="13" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="9"/>
+      <c r="H23" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="8">
+        <v>40626</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="N23" s="26">
+        <v>1</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>60</v>
+      </c>
       <c r="P23" s="9"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" ht="28">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -2533,14 +2714,30 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="9"/>
+      <c r="H24" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" s="8">
+        <v>40626</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M24" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" s="26">
+        <v>1</v>
+      </c>
+      <c r="O24" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="P24" s="9"/>
     </row>
     <row r="25" spans="1:16">
@@ -2549,18 +2746,34 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="13" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="9"/>
+      <c r="H25" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="8">
+        <v>40626</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M25" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N25" s="26">
+        <v>1</v>
+      </c>
+      <c r="O25" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="P25" s="9"/>
     </row>
     <row r="26" spans="1:16">
@@ -2571,14 +2784,14 @@
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="13"/>
+      <c r="H26" s="29"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="9"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="16"/>
       <c r="P26" s="9"/>
     </row>
     <row r="27" spans="1:16">
@@ -2586,18 +2799,18 @@
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="19" t="s">
-        <v>22</v>
+      <c r="E27" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="7"/>
+      <c r="H27" s="29"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
-      <c r="N27" s="27"/>
+      <c r="N27" s="26"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
     </row>
@@ -2615,7 +2828,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
-      <c r="N28" s="27"/>
+      <c r="N28" s="26"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
     </row>
@@ -2624,7 +2837,7 @@
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -2635,7 +2848,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
-      <c r="N29" s="27"/>
+      <c r="N29" s="26"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
     </row>
@@ -2653,7 +2866,7 @@
       <c r="K30" s="7"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
-      <c r="N30" s="27"/>
+      <c r="N30" s="26"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
     </row>
@@ -2663,7 +2876,7 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="13" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="10"/>
@@ -2673,7 +2886,7 @@
       <c r="K31" s="7"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="27"/>
+      <c r="N31" s="26"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
     </row>
@@ -2691,7 +2904,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
-      <c r="N32" s="27"/>
+      <c r="N32" s="26"/>
       <c r="O32" s="9"/>
       <c r="P32" s="9"/>
     </row>
@@ -2702,7 +2915,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="12" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="12"/>
@@ -2711,7 +2924,7 @@
       <c r="K33" s="12"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
-      <c r="N33" s="27"/>
+      <c r="N33" s="26"/>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
     </row>
@@ -2729,7 +2942,7 @@
       <c r="K34" s="12"/>
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
-      <c r="N34" s="27"/>
+      <c r="N34" s="26"/>
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
     </row>
@@ -2740,7 +2953,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="12" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="12"/>
@@ -2749,7 +2962,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
-      <c r="N35" s="27"/>
+      <c r="N35" s="26"/>
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
     </row>
@@ -2767,7 +2980,7 @@
       <c r="K36" s="12"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
-      <c r="N36" s="27"/>
+      <c r="N36" s="26"/>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
     </row>
@@ -2778,7 +2991,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="12" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="12"/>
@@ -2787,7 +3000,7 @@
       <c r="K37" s="12"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
-      <c r="N37" s="27"/>
+      <c r="N37" s="26"/>
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
     </row>
@@ -2805,7 +3018,7 @@
       <c r="K38" s="12"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
-      <c r="N38" s="27"/>
+      <c r="N38" s="26"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
     </row>
@@ -2815,7 +3028,7 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="13" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="10"/>
@@ -2825,13 +3038,13 @@
       <c r="K39" s="7"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
-      <c r="N39" s="27"/>
+      <c r="N39" s="26"/>
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
     </row>
     <row r="41" spans="1:16">
       <c r="E41" s="16" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2865,7 +3078,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -2883,7 +3095,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
28/03/2011 - 00.11 - Update for this evening. See README Signed-off-by: Dave Russell <dave.aj.russell@gmail.com>
</commit_message>
<xml_diff>
--- a/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
+++ b/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14600"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="14595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,11 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="138">
-  <si>
-    <t>Visio drawing containing some new designs which were not included in BHH document, which are required for our implementation</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="146">
   <si>
     <t>AnnotatedRequirements.docx</t>
     <phoneticPr fontId="7" type="noConversion"/>
@@ -578,6 +574,33 @@
   </si>
   <si>
     <t>staffs-ppsp-repo</t>
+  </si>
+  <si>
+    <t>I23</t>
+  </si>
+  <si>
+    <t>NewDesigns.png</t>
+  </si>
+  <si>
+    <t>Visio drawing containing some simple screen designs which were not included in the original spec</t>
+  </si>
+  <si>
+    <t>PNG format of the simple new designs</t>
+  </si>
+  <si>
+    <t>V21</t>
+  </si>
+  <si>
+    <t>I24</t>
+  </si>
+  <si>
+    <t>QualityAuditTemplate.docx</t>
+  </si>
+  <si>
+    <t>Template for the quality audit doucment</t>
+  </si>
+  <si>
+    <t>V22</t>
   </si>
 </sst>
 </file>
@@ -805,6 +828,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -812,9 +838,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -847,8 +870,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2108200" y="477307"/>
-          <a:ext cx="218440" cy="268553"/>
+          <a:off x="1841500" y="485774"/>
+          <a:ext cx="218440" cy="277019"/>
           <a:chOff x="1640840" y="238760"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -937,8 +960,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3110442" y="833967"/>
-          <a:ext cx="377825" cy="283633"/>
+          <a:off x="2720975" y="850900"/>
+          <a:ext cx="377825" cy="292100"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1027,8 +1050,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3119967" y="1938867"/>
-          <a:ext cx="353060" cy="258180"/>
+          <a:off x="2730500" y="1981200"/>
+          <a:ext cx="353060" cy="262414"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1117,8 +1140,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4556124" y="2339974"/>
-          <a:ext cx="742951" cy="239766"/>
+          <a:off x="3984624" y="2390774"/>
+          <a:ext cx="742951" cy="243999"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1207,8 +1230,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4660900" y="3467100"/>
-          <a:ext cx="666749" cy="230240"/>
+          <a:off x="4089400" y="3543300"/>
+          <a:ext cx="666749" cy="234473"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1297,8 +1320,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4613275" y="5470524"/>
-          <a:ext cx="742950" cy="248656"/>
+          <a:off x="4041775" y="5610224"/>
+          <a:ext cx="742950" cy="252889"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1387,8 +1410,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7084483" y="5862108"/>
-          <a:ext cx="551180" cy="239766"/>
+          <a:off x="6191250" y="6010275"/>
+          <a:ext cx="551180" cy="243999"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1524,8 +1547,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4527550" y="1203324"/>
-          <a:ext cx="790575" cy="243418"/>
+          <a:off x="3956050" y="1228724"/>
+          <a:ext cx="790575" cy="247651"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
         </a:xfrm>
@@ -1881,108 +1904,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="1"/>
-    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1"/>
+    <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="61" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="33.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="73.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="12.5" style="1"/>
+    <col min="10" max="10" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="73.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="12.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16">
-      <c r="A2" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="A2" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="M2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K3" s="8">
         <v>40620</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N3" s="26">
         <v>1.3</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1994,69 +2017,69 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K4" s="30">
         <v>40620</v>
       </c>
       <c r="L4" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M4" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N4" s="32">
         <v>1.1000000000000001</v>
       </c>
       <c r="O4" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P4" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="6"/>
-      <c r="B5" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="34"/>
+      <c r="B5" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="35"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K5" s="8">
         <v>40620</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N5" s="26">
         <v>1.1000000000000001</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -2068,31 +2091,31 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="J6" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K6" s="8">
         <v>40620</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N6" s="26">
         <v>1</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -2100,37 +2123,37 @@
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="J7" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K7" s="8">
         <v>40620</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N7" s="26">
         <v>1</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -2142,31 +2165,31 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K8" s="8">
         <v>40620</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N8" s="26">
         <v>1</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -2174,36 +2197,36 @@
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="E9" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K9" s="8">
         <v>40620</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N9" s="26">
         <v>1</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2215,69 +2238,69 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K10" s="8">
         <v>40620</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N10" s="26">
         <v>1</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="6"/>
-      <c r="B11" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="34"/>
+      <c r="B11" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="35"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K11" s="8">
         <v>40620</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N11" s="26">
         <v>1</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2289,31 +2312,31 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K12" s="8">
         <v>40620</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N12" s="26">
         <v>1</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2321,37 +2344,37 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="J13" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="8">
         <v>40621</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N13" s="26">
         <v>1.1000000000000001</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2363,31 +2386,31 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="K14" s="8">
         <v>40622</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N14" s="26">
         <v>1</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2396,33 +2419,33 @@
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
       <c r="E15" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
       <c r="H15" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K15" s="21">
         <v>40623</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N15" s="27">
         <v>1.1000000000000001</v>
       </c>
       <c r="O15" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P15" s="22"/>
     </row>
@@ -2435,28 +2458,28 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="J16" s="23" t="s">
         <v>112</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>113</v>
       </c>
       <c r="K16" s="21">
         <v>40623</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N16" s="27">
         <v>1.2</v>
       </c>
       <c r="O16" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P16" s="22"/>
     </row>
@@ -2466,33 +2489,33 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="J17" s="23" t="s">
         <v>116</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>117</v>
       </c>
       <c r="K17" s="21">
         <v>40625</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N17" s="27">
         <v>1.2</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P17" s="22"/>
     </row>
@@ -2505,28 +2528,28 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K18" s="8">
         <v>40626</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N18" s="26">
         <v>1.6</v>
       </c>
       <c r="O18" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P18" s="9"/>
     </row>
@@ -2535,34 +2558,34 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="I19" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="I19" s="29" t="s">
+      <c r="J19" s="29" t="s">
         <v>124</v>
-      </c>
-      <c r="J19" s="29" t="s">
-        <v>125</v>
       </c>
       <c r="K19" s="8">
         <v>40625</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M19" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N19" s="26">
         <v>1.1000000000000001</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P19" s="9"/>
     </row>
@@ -2575,28 +2598,28 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="I20" s="29" t="s">
+      <c r="J20" s="29" t="s">
         <v>88</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>89</v>
       </c>
       <c r="K20" s="8">
         <v>40626</v>
       </c>
       <c r="L20" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="M20" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="M20" s="16" t="s">
+      <c r="N20" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O20" s="16" t="s">
         <v>91</v>
-      </c>
-      <c r="N20" s="26">
-        <v>1</v>
-      </c>
-      <c r="O20" s="16" t="s">
-        <v>92</v>
       </c>
       <c r="P20" s="9"/>
     </row>
@@ -2606,33 +2629,33 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="10"/>
       <c r="H21" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I21" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="29" t="s">
         <v>49</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>50</v>
       </c>
       <c r="K21" s="8">
         <v>40630</v>
       </c>
       <c r="L21" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M21" s="16" t="s">
         <v>51</v>
-      </c>
-      <c r="M21" s="16" t="s">
-        <v>52</v>
       </c>
       <c r="N21" s="26">
         <v>1</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P21" s="9"/>
     </row>
@@ -2645,28 +2668,28 @@
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I22" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="29" t="s">
         <v>54</v>
-      </c>
-      <c r="J22" s="29" t="s">
-        <v>55</v>
       </c>
       <c r="K22" s="8">
         <v>40629</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N22" s="26">
         <v>1</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P22" s="9"/>
     </row>
@@ -2676,37 +2699,37 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="10"/>
       <c r="H23" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J23" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K23" s="8">
         <v>40626</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N23" s="26">
         <v>1</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P23" s="9"/>
     </row>
-    <row r="24" spans="1:16" ht="28">
+    <row r="24" spans="1:16" ht="30">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -2715,28 +2738,28 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J24" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K24" s="8">
         <v>40626</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="M24" s="37" t="s">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="M24" s="34" t="s">
+        <v>139</v>
       </c>
       <c r="N24" s="26">
         <v>1</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P24" s="9"/>
     </row>
@@ -2746,33 +2769,33 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="10"/>
       <c r="H25" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I25" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="29" t="s">
         <v>1</v>
-      </c>
-      <c r="J25" s="29" t="s">
-        <v>2</v>
       </c>
       <c r="K25" s="8">
         <v>40626</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N25" s="26">
         <v>1</v>
       </c>
       <c r="O25" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P25" s="9"/>
     </row>
@@ -2784,14 +2807,30 @@
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="16"/>
+      <c r="H26" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="K26" s="8">
+        <v>40630</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="N26" s="26">
+        <v>1</v>
+      </c>
+      <c r="O26" s="16" t="s">
+        <v>141</v>
+      </c>
       <c r="P26" s="9"/>
     </row>
     <row r="27" spans="1:16">
@@ -2800,18 +2839,34 @@
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="9"/>
+      <c r="H27" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K27" s="8">
+        <v>40630</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="N27" s="26">
+        <v>1</v>
+      </c>
+      <c r="O27" s="16" t="s">
+        <v>145</v>
+      </c>
       <c r="P27" s="9"/>
     </row>
     <row r="28" spans="1:16">
@@ -2837,7 +2892,7 @@
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -2876,7 +2931,7 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="10"/>
@@ -2915,7 +2970,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="12"/>
@@ -2953,7 +3008,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="12"/>
@@ -2991,7 +3046,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="12"/>
@@ -3028,7 +3083,7 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="10"/>
@@ -3044,7 +3099,7 @@
     </row>
     <row r="41" spans="1:16">
       <c r="E41" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3071,12 +3126,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3088,12 +3143,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
29/03/2011 - 21.29 - See README for change log Signed-off-by: Dave Russell <dave.aj.russell@gmail.com>
</commit_message>
<xml_diff>
--- a/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
+++ b/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
@@ -27,7 +27,7 @@
     <author>David Russell</author>
   </authors>
   <commentList>
-    <comment ref="O14" authorId="0">
+    <comment ref="P14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O21" authorId="1">
+    <comment ref="P21" authorId="1">
       <text>
         <r>
           <rPr>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="160">
   <si>
     <t>AnnotatedRequirements.docx</t>
     <phoneticPr fontId="7" type="noConversion"/>
@@ -601,6 +601,48 @@
   </si>
   <si>
     <t>V22</t>
+  </si>
+  <si>
+    <t>2.3.4_Testing</t>
+  </si>
+  <si>
+    <t>2.3.1_QualityDocuments</t>
+  </si>
+  <si>
+    <t>2.3.5_UserSupport</t>
+  </si>
+  <si>
+    <t>Ver_1.6</t>
+  </si>
+  <si>
+    <t>I25</t>
+  </si>
+  <si>
+    <t>FinalDocument.docx</t>
+  </si>
+  <si>
+    <t>Final Document</t>
+  </si>
+  <si>
+    <t>V23</t>
+  </si>
+  <si>
+    <t>I26</t>
+  </si>
+  <si>
+    <t>basis testing functions.docx</t>
+  </si>
+  <si>
+    <t>I27</t>
+  </si>
+  <si>
+    <t>TestTemplate.docx</t>
+  </si>
+  <si>
+    <t>James's basis path test flow graphs</t>
+  </si>
+  <si>
+    <t>Template for tests to be recorded on</t>
   </si>
 </sst>
 </file>
@@ -767,7 +809,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -838,6 +880,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -870,7 +918,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1841500" y="485774"/>
+          <a:off x="1845129" y="485774"/>
           <a:ext cx="218440" cy="277019"/>
           <a:chOff x="1640840" y="238760"/>
           <a:chExt cx="574040" cy="249714"/>
@@ -960,7 +1008,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2720975" y="850900"/>
+          <a:off x="2722789" y="850900"/>
           <a:ext cx="377825" cy="292100"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
@@ -1050,7 +1098,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2730500" y="1981200"/>
+          <a:off x="2732314" y="1981200"/>
           <a:ext cx="353060" cy="262414"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
@@ -1140,7 +1188,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3984624" y="2390774"/>
+          <a:off x="3990974" y="2390774"/>
           <a:ext cx="742951" cy="243999"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
@@ -1214,13 +1262,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>857249</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>158273</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1230,7 +1278,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4089400" y="3543300"/>
+          <a:off x="4095750" y="4114800"/>
           <a:ext cx="666749" cy="234473"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
@@ -1304,13 +1352,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>885825</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>148113</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1320,7 +1368,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4041775" y="5610224"/>
+          <a:off x="4048125" y="6181724"/>
           <a:ext cx="742950" cy="252889"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
@@ -1358,96 +1406,6 @@
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
           <xdr:cNvPr id="19" name="Straight Arrow Connector 18"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="5400000">
-            <a:off x="436880" y="124460"/>
-            <a:ext cx="248920" cy="1588"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:tailEnd type="arrow"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>608330</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>158274</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="20" name="Group 19"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="6191250" y="6010275"/>
-          <a:ext cx="551180" cy="243999"/>
-          <a:chOff x="0" y="0"/>
-          <a:chExt cx="574040" cy="249714"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="21" name="Straight Connector 20"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="574040" cy="1588"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="22" name="Straight Arrow Connector 21"/>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1547,7 +1505,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3956050" y="1228724"/>
+          <a:off x="3962400" y="1228724"/>
           <a:ext cx="790575" cy="247651"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
@@ -1585,6 +1543,96 @@
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
           <xdr:cNvPr id="29" name="Straight Arrow Connector 28"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="436880" y="124460"/>
+            <a:ext cx="248920" cy="1588"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>156482</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>107496</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>708933</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="30" name="Group 29"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6293303" y="2774496"/>
+          <a:ext cx="742951" cy="232683"/>
+          <a:chOff x="0" y="0"/>
+          <a:chExt cx="574040" cy="249714"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="31" name="Straight Connector 30"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="574040" cy="1588"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="32" name="Straight Arrow Connector 31"/>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1905,10 +1953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:P41"/>
+  <dimension ref="A2:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15"/>
@@ -1916,23 +1964,24 @@
     <col min="1" max="1" width="12.42578125" style="1"/>
     <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="73.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="12.42578125" style="1"/>
+    <col min="6" max="6" width="2.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="61" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="73.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="12.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="36" t="s">
         <v>63</v>
       </c>
@@ -1941,36 +1990,37 @@
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
       <c r="F2" s="37"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="37"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="O2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="P2" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="Q2" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" s="35" t="s">
         <v>136</v>
       </c>
@@ -1980,35 +2030,36 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="8">
+      <c r="L3" s="8">
         <v>40620</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="26">
-        <v>1.3</v>
-      </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="26">
+        <v>2.4</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2016,35 +2067,36 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="J4" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="K4" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="30">
+      <c r="L4" s="30">
         <v>40620</v>
       </c>
-      <c r="L4" s="31" t="s">
+      <c r="M4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="31" t="s">
+      <c r="N4" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="32">
+      <c r="O4" s="32">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O4" s="31" t="s">
+      <c r="P4" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="P4" s="31" t="s">
+      <c r="Q4" s="31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" s="6"/>
       <c r="B5" s="35" t="s">
         <v>4</v>
@@ -2054,35 +2106,36 @@
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="10"/>
+      <c r="I5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="K5" s="8">
+      <c r="L5" s="8">
         <v>40620</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="M5" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="N5" s="26">
+      <c r="O5" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="P5" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="Q5" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" s="6"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -2090,35 +2143,36 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="10"/>
+      <c r="I6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="K6" s="8">
+      <c r="L6" s="8">
         <v>40620</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="M6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="N6" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="26">
+      <c r="O6" s="26">
         <v>1</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="P6" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="Q6" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" s="6"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -2128,35 +2182,36 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="10"/>
+      <c r="I7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="K7" s="8">
+      <c r="L7" s="8">
         <v>40620</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="M7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="N7" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="N7" s="26">
+      <c r="O7" s="26">
         <v>1</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="P7" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="Q7" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" s="6"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -2164,72 +2219,74 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="10"/>
+      <c r="I8" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="K8" s="8">
+      <c r="L8" s="8">
         <v>40620</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="M8" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="N8" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="N8" s="26">
+      <c r="O8" s="26">
         <v>1</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="P8" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="P8" s="16" t="s">
+      <c r="Q8" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" s="6"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="E9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10"/>
+      <c r="I9" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="K9" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="K9" s="8">
+      <c r="L9" s="21">
         <v>40620</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="M9" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="N9" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="26">
+      <c r="O9" s="27">
         <v>1</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="P9" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="Q9" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" s="6"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2237,35 +2294,36 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="10"/>
+      <c r="I10" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="J10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="K10" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="K10" s="8">
+      <c r="L10" s="8">
         <v>40620</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="M10" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="N10" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="N10" s="26">
+      <c r="O10" s="26">
         <v>1</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="P10" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="P10" s="16" t="s">
+      <c r="Q10" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11" s="6"/>
       <c r="B11" s="35" t="s">
         <v>5</v>
@@ -2275,35 +2333,36 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="10"/>
+      <c r="I11" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="K11" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="K11" s="8">
+      <c r="L11" s="8">
         <v>40620</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="M11" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="N11" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="N11" s="26">
-        <v>1</v>
-      </c>
-      <c r="O11" s="16" t="s">
+      <c r="O11" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P11" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="16" t="s">
+      <c r="Q11" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="A12" s="6"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -2311,35 +2370,36 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="J12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="K12" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="K12" s="8">
+      <c r="L12" s="8">
         <v>40620</v>
       </c>
-      <c r="L12" s="16" t="s">
+      <c r="M12" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="N12" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="N12" s="26">
+      <c r="O12" s="26">
         <v>1</v>
       </c>
-      <c r="O12" s="16" t="s">
+      <c r="P12" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="P12" s="16" t="s">
+      <c r="Q12" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2347,73 +2407,75 @@
         <v>6</v>
       </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="10"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="6"/>
+      <c r="I13" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="J13" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="K13" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="K13" s="8">
+      <c r="L13" s="8">
         <v>40621</v>
       </c>
-      <c r="L13" s="16" t="s">
-        <v>15</v>
-      </c>
       <c r="M13" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="N13" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="26">
+      <c r="O13" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O13" s="16" t="s">
+      <c r="P13" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="P13" s="16" t="s">
+      <c r="Q13" s="16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6"/>
+      <c r="I14" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="J14" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="K14" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="K14" s="8">
+      <c r="L14" s="8">
         <v>40622</v>
       </c>
-      <c r="L14" s="16" t="s">
+      <c r="M14" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="M14" s="16" t="s">
+      <c r="N14" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="N14" s="26">
-        <v>1</v>
-      </c>
-      <c r="O14" s="16" t="s">
+      <c r="O14" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P14" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="P14" s="16" t="s">
+      <c r="Q14" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
@@ -2421,698 +2483,791 @@
       <c r="E15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="19" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="J15" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="K15" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="21">
+      <c r="L15" s="21">
         <v>40623</v>
       </c>
-      <c r="L15" s="22" t="s">
+      <c r="M15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="22" t="s">
+      <c r="N15" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="N15" s="27">
+      <c r="O15" s="27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O15" s="22" t="s">
+      <c r="P15" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="P15" s="22"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15" s="22"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="23" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="J16" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="K16" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="K16" s="21">
+      <c r="L16" s="21">
         <v>40623</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="M16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="N16" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="N16" s="27">
+      <c r="O16" s="27">
         <v>1.2</v>
       </c>
-      <c r="O16" s="22" t="s">
+      <c r="P16" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="P16" s="22"/>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" s="22"/>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="L17" s="21">
+        <v>40625</v>
+      </c>
+      <c r="M17" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="K17" s="21">
-        <v>40625</v>
-      </c>
-      <c r="L17" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="M17" s="22" t="s">
+      <c r="N17" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="N17" s="27">
+      <c r="O17" s="27">
         <v>1.2</v>
       </c>
-      <c r="O17" s="22" t="s">
+      <c r="P17" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="P17" s="22"/>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17" s="22"/>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="J18" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="K18" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="K18" s="8">
+      <c r="L18" s="8">
         <v>40626</v>
       </c>
-      <c r="L18" s="16" t="s">
+      <c r="M18" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="16" t="s">
+      <c r="N18" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="N18" s="26">
+      <c r="O18" s="26">
         <v>1.6</v>
       </c>
-      <c r="O18" s="16" t="s">
+      <c r="P18" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="P18" s="9"/>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18" s="9"/>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="14"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="29" t="s">
+      <c r="H19" s="6"/>
+      <c r="I19" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="I19" s="29" t="s">
+      <c r="J19" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="J19" s="29" t="s">
+      <c r="K19" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="K19" s="8">
+      <c r="L19" s="8">
         <v>40625</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="M19" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="M19" s="33" t="s">
+      <c r="N19" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="N19" s="26">
+      <c r="O19" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O19" s="16" t="s">
+      <c r="P19" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="P19" s="9"/>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19" s="9"/>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="14"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="6"/>
+      <c r="I20" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="I20" s="29" t="s">
+      <c r="J20" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="K20" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="K20" s="8">
+      <c r="L20" s="8">
         <v>40626</v>
       </c>
-      <c r="L20" s="16" t="s">
+      <c r="M20" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="M20" s="16" t="s">
+      <c r="N20" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="N20" s="26">
+      <c r="O20" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O20" s="16" t="s">
+      <c r="P20" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="P20" s="9"/>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20" s="9"/>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="29" t="s">
+      <c r="E21" s="6"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="29" t="s">
+      <c r="J21" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="K21" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="K21" s="8">
+      <c r="L21" s="8">
         <v>40630</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="M21" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="M21" s="16" t="s">
+      <c r="N21" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="N21" s="26">
+      <c r="O21" s="26">
         <v>1</v>
       </c>
-      <c r="O21" s="16" t="s">
+      <c r="P21" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="P21" s="9"/>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21" s="9"/>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="29" t="s">
+      <c r="D22" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="29" t="s">
+      <c r="J22" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="K22" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="K22" s="8">
+      <c r="L22" s="8">
         <v>40629</v>
       </c>
-      <c r="L22" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="M22" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="N22" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="N22" s="26">
-        <v>1</v>
-      </c>
-      <c r="O22" s="16" t="s">
+      <c r="O22" s="26">
+        <v>1.3</v>
+      </c>
+      <c r="P22" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="P22" s="9"/>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22" s="9"/>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="29" t="s">
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="29" t="s">
+      <c r="J23" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J23" s="29" t="s">
+      <c r="K23" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="K23" s="8">
+      <c r="L23" s="8">
         <v>40626</v>
       </c>
-      <c r="L23" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="M23" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="N23" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="N23" s="26">
-        <v>1</v>
-      </c>
-      <c r="O23" s="16" t="s">
+      <c r="O23" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="P23" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="P23" s="9"/>
-    </row>
-    <row r="24" spans="1:16" ht="30">
+      <c r="Q23" s="9"/>
+    </row>
+    <row r="24" spans="1:17" ht="30">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="29" t="s">
+      <c r="E24" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="29" t="s">
+      <c r="J24" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="J24" s="29" t="s">
+      <c r="K24" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="8">
+      <c r="L24" s="8">
         <v>40626</v>
       </c>
-      <c r="L24" s="16" t="s">
+      <c r="M24" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="M24" s="34" t="s">
+      <c r="N24" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="N24" s="26">
+      <c r="O24" s="26">
         <v>1</v>
       </c>
-      <c r="O24" s="16" t="s">
+      <c r="P24" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="P24" s="9"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="Q24" s="9"/>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="29" t="s">
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="I25" s="29" t="s">
+      <c r="J25" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J25" s="29" t="s">
+      <c r="K25" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="K25" s="8">
+      <c r="L25" s="8">
         <v>40626</v>
       </c>
-      <c r="L25" s="16" t="s">
+      <c r="M25" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="M25" s="16" t="s">
+      <c r="N25" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="N25" s="26">
+      <c r="O25" s="26">
         <v>1</v>
       </c>
-      <c r="O25" s="16" t="s">
+      <c r="P25" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="P25" s="9"/>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="9"/>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="F26" s="14"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="29" t="s">
+      <c r="G26" s="14"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="J26" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="K26" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="K26" s="8">
+      <c r="L26" s="8">
         <v>40630</v>
       </c>
-      <c r="L26" s="16" t="s">
+      <c r="M26" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="M26" s="16" t="s">
+      <c r="N26" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="N26" s="26">
+      <c r="O26" s="26">
         <v>1</v>
       </c>
-      <c r="O26" s="16" t="s">
+      <c r="P26" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="P26" s="9"/>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" s="9"/>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="29" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="J27" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J27" s="7" t="s">
+      <c r="K27" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="K27" s="8">
+      <c r="L27" s="8">
         <v>40630</v>
       </c>
-      <c r="L27" s="16" t="s">
-        <v>15</v>
-      </c>
       <c r="M27" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="N27" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="N27" s="26">
-        <v>1</v>
-      </c>
-      <c r="O27" s="16" t="s">
+      <c r="O27" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P27" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="P27" s="9"/>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27" s="9"/>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+      <c r="E28" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="39"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="H28" s="6"/>
+      <c r="I28" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L28" s="8">
+        <v>40629</v>
+      </c>
+      <c r="M28" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N28" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="O28" s="26">
+        <v>1.4</v>
+      </c>
+      <c r="P28" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q28" s="9"/>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
-      <c r="D29" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="H29" s="6"/>
+      <c r="I29" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L29" s="8">
+        <v>40631</v>
+      </c>
+      <c r="M29" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="N29" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="O29" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P29" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q29" s="9"/>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="E30" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="H30" s="6"/>
+      <c r="I30" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L30" s="8">
+        <v>40631</v>
+      </c>
+      <c r="M30" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="N30" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="O30" s="26">
+        <v>1</v>
+      </c>
+      <c r="P30" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q30" s="9"/>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="7"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="13"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
-      <c r="L31" s="9"/>
+      <c r="L31" s="7"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="26"/>
       <c r="P31" s="9"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31" s="9"/>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="7"/>
+      <c r="D32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="13"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
-      <c r="L32" s="9"/>
+      <c r="L32" s="7"/>
       <c r="M32" s="9"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="26"/>
       <c r="P32" s="9"/>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="Q32" s="9"/>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="11"/>
-      <c r="H33" s="12"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="11"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
-      <c r="L33" s="9"/>
+      <c r="L33" s="12"/>
       <c r="M33" s="9"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="26"/>
       <c r="P33" s="9"/>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33" s="9"/>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="12"/>
+      <c r="E34" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="42"/>
+      <c r="G34" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="11"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
-      <c r="L34" s="9"/>
+      <c r="L34" s="12"/>
       <c r="M34" s="9"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="26"/>
       <c r="P34" s="9"/>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="Q34" s="9"/>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="42"/>
       <c r="G35" s="11"/>
-      <c r="H35" s="12"/>
+      <c r="H35" s="11"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
-      <c r="L35" s="9"/>
+      <c r="L35" s="12"/>
       <c r="M35" s="9"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="26"/>
       <c r="P35" s="9"/>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="Q35" s="9"/>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="12"/>
+      <c r="E36" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F36" s="14"/>
+      <c r="G36" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="11"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
-      <c r="L36" s="9"/>
+      <c r="L36" s="12"/>
       <c r="M36" s="9"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="26"/>
       <c r="P36" s="9"/>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="Q36" s="9"/>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="F37" s="43"/>
       <c r="G37" s="11"/>
-      <c r="H37" s="12"/>
+      <c r="H37" s="11"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
-      <c r="L37" s="9"/>
+      <c r="L37" s="12"/>
       <c r="M37" s="9"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="26"/>
       <c r="P37" s="9"/>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="Q37" s="9"/>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="12"/>
+      <c r="E38" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="41"/>
+      <c r="G38" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="11"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
-      <c r="L38" s="9"/>
+      <c r="L38" s="12"/>
       <c r="M38" s="9"/>
-      <c r="N38" s="26"/>
-      <c r="O38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="26"/>
       <c r="P38" s="9"/>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38" s="9"/>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="14"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="7"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="13"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
-      <c r="L39" s="9"/>
+      <c r="L39" s="7"/>
       <c r="M39" s="9"/>
-      <c r="N39" s="26"/>
-      <c r="O39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="26"/>
       <c r="P39" s="9"/>
-    </row>
-    <row r="41" spans="1:16">
-      <c r="E41" s="16" t="s">
+      <c r="Q39" s="9"/>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="D40" s="6"/>
+      <c r="E40" s="16" t="s">
         <v>62</v>
+      </c>
+      <c r="F40" s="41"/>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="D42" s="6"/>
+      <c r="E42" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="41"/>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="E44" s="16" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1"/>
-    <hyperlink ref="O2" r:id="rId2"/>
+    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink ref="P2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>

</xml_diff>

<commit_message>
Commit of today's work 30/03/2011 - 23.42 Signed-off-by: Dave Russell <dave.aj.russell@gmail.com>
</commit_message>
<xml_diff>
--- a/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
+++ b/2_Part2_Implementation/2.2_Control_Logs/2.2.2_RepoIndexes/Index.xlsx
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P21" authorId="1">
+    <comment ref="P22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -80,11 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="160">
-  <si>
-    <t>AnnotatedRequirements.docx</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="185">
   <si>
     <t>Scott Dennison</t>
     <phoneticPr fontId="7" type="noConversion"/>
@@ -94,10 +90,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>TestCases.docx</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>1_Part1_Specification/Design</t>
   </si>
   <si>
@@ -164,9 +156,6 @@
     <t>Index log of all changes to all directories and content for the project</t>
   </si>
   <si>
-    <t>VC3</t>
-  </si>
-  <si>
     <t>Index ID</t>
   </si>
   <si>
@@ -182,9 +171,6 @@
     <t>Current Version</t>
   </si>
   <si>
-    <t>VC1, VC2, VC4</t>
-  </si>
-  <si>
     <t>Date of Creation</t>
   </si>
   <si>
@@ -228,10 +214,6 @@
   </si>
   <si>
     <t>V20</t>
-  </si>
-  <si>
-    <t>DesignReview.docx</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>David Russell</t>
@@ -250,10 +232,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>BasisPathTesting.docx</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>David Russell, James Nightingale</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -278,10 +256,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>NewDesigns.vsd</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Partner groups revised requirements specification </t>
   </si>
   <si>
@@ -306,21 +280,9 @@
     <t>I10</t>
   </si>
   <si>
-    <t>Plan.docx</t>
-  </si>
-  <si>
     <t>QualityAssurance.docx</t>
   </si>
   <si>
-    <t>Requirements.docx</t>
-  </si>
-  <si>
-    <t>ResourceAllocation.docx</t>
-  </si>
-  <si>
-    <t>Strategy.docx</t>
-  </si>
-  <si>
     <t>Document outlining the plan of the implementation phase</t>
   </si>
   <si>
@@ -342,9 +304,6 @@
     <t>I11</t>
   </si>
   <si>
-    <t>CodingStandards.docx</t>
-  </si>
-  <si>
     <t>Document establish coding standards for all developers</t>
   </si>
   <si>
@@ -352,19 +311,12 @@
   </si>
   <si>
     <t>I12</t>
-  </si>
-  <si>
-    <t>David Russell, Scott Dennison</t>
   </si>
   <si>
     <t>I17</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>RequirementsTracing.docx</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>David Russell</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -388,12 +340,6 @@
   </si>
   <si>
     <t>CommLog01.docx</t>
-  </si>
-  <si>
-    <t>VC1, VC4</t>
-  </si>
-  <si>
-    <t>VC1,VC3, VC4, VC7</t>
   </si>
   <si>
     <t>SWVersion ID</t>
@@ -489,29 +435,11 @@
     <t>Group</t>
   </si>
   <si>
-    <r>
-      <t>Ver_1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>I16</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SWVersionControl_NEW.xlsx</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scott Dennison</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -579,9 +507,6 @@
     <t>I23</t>
   </si>
   <si>
-    <t>NewDesigns.png</t>
-  </si>
-  <si>
     <t>Visio drawing containing some simple screen designs which were not included in the original spec</t>
   </si>
   <si>
@@ -643,6 +568,149 @@
   </si>
   <si>
     <t>Template for tests to be recorded on</t>
+  </si>
+  <si>
+    <t>I28</t>
+  </si>
+  <si>
+    <t>James Nightingale, Amanda Patterson</t>
+  </si>
+  <si>
+    <r>
+      <t>Ver_1.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <t>Amanda Patterson</t>
+  </si>
+  <si>
+    <t>Scott Dennison, David Russell</t>
+  </si>
+  <si>
+    <t>The user manual for the system</t>
+  </si>
+  <si>
+    <t>V24</t>
+  </si>
+  <si>
+    <t>I29</t>
+  </si>
+  <si>
+    <t>Ver_1.7</t>
+  </si>
+  <si>
+    <t>David Russell, James Nightingale</t>
+  </si>
+  <si>
+    <t>New version of the implementation</t>
+  </si>
+  <si>
+    <t>V25</t>
+  </si>
+  <si>
+    <t>01_Plan.docx</t>
+  </si>
+  <si>
+    <t>02_Strategy.docx</t>
+  </si>
+  <si>
+    <t>03_DesignReview.docx</t>
+  </si>
+  <si>
+    <t>04_Requirements.docx</t>
+  </si>
+  <si>
+    <t>05_ResourceAllocation.docx</t>
+  </si>
+  <si>
+    <t>06_AnnotatedRequirements.docx</t>
+  </si>
+  <si>
+    <t>07_NewDesigns.png</t>
+  </si>
+  <si>
+    <t>07_NewDesigns.vsd</t>
+  </si>
+  <si>
+    <t>08_QualityAssurance.docx</t>
+  </si>
+  <si>
+    <t>01_UserManual.docx</t>
+  </si>
+  <si>
+    <t>I30</t>
+  </si>
+  <si>
+    <t>01_CodingStandards.docx</t>
+  </si>
+  <si>
+    <t>02_TestingStandards.docx</t>
+  </si>
+  <si>
+    <t>01_RequirementsTracing.docx</t>
+  </si>
+  <si>
+    <t>01_TestCases.docx</t>
+  </si>
+  <si>
+    <t>02_BasisPathTesting.docx</t>
+  </si>
+  <si>
+    <t>I31</t>
+  </si>
+  <si>
+    <t>03_UnitTests.docx</t>
+  </si>
+  <si>
+    <t>I32</t>
+  </si>
+  <si>
+    <t>04_BlackBoxTesting</t>
+  </si>
+  <si>
+    <t>Amanda Patterson, James Nightingale</t>
+  </si>
+  <si>
+    <t>I33</t>
+  </si>
+  <si>
+    <t>black box u.docx</t>
+  </si>
+  <si>
+    <t>I34</t>
+  </si>
+  <si>
+    <t>blackboxtestdata.docx</t>
+  </si>
+  <si>
+    <t>Testing standards. These set a base line for testing standards for the project</t>
+  </si>
+  <si>
+    <t>V26</t>
+  </si>
+  <si>
+    <t>Recorded unit tests of all classes in the implementation</t>
+  </si>
+  <si>
+    <t>V27</t>
+  </si>
+  <si>
+    <t>Recorded black box test results</t>
+  </si>
+  <si>
+    <t>V28</t>
+  </si>
+  <si>
+    <t>Document storing some black box test results, to be added to the final document</t>
   </si>
 </sst>
 </file>
@@ -809,7 +877,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -824,7 +892,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -847,7 +914,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -864,7 +930,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -873,6 +938,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -880,12 +951,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1262,13 +1348,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>857249</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>158273</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1278,7 +1364,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4095750" y="4114800"/>
+          <a:off x="4095750" y="4305300"/>
           <a:ext cx="666749" cy="234473"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
@@ -1352,13 +1438,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>885825</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>148113</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1368,7 +1454,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4048125" y="6181724"/>
+          <a:off x="4048125" y="6372224"/>
           <a:ext cx="742950" cy="252889"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="574040" cy="249714"/>
@@ -1953,10 +2039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:Q44"/>
+  <dimension ref="A2:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15"/>
@@ -1970,61 +2056,61 @@
     <col min="7" max="7" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="61" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="38.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="73.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="46" customWidth="1"/>
+    <col min="13" max="13" width="35.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="94.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="12.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17">
-      <c r="A2" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="A2" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
       <c r="H2" s="2"/>
       <c r="I2" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>97</v>
+      <c r="O2" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" s="35"/>
+      <c r="A3" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="38"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
@@ -2032,32 +2118,30 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="8">
+        <v>68</v>
+      </c>
+      <c r="L3" s="42">
         <v>40620</v>
       </c>
-      <c r="M3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="26">
+      <c r="M3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="24">
         <v>2.4</v>
       </c>
-      <c r="P3" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>32</v>
-      </c>
+      <c r="P3" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q3" s="15"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="6"/>
@@ -2068,1193 +2152,1318 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" s="30">
+      <c r="I4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="43">
         <v>40620</v>
       </c>
-      <c r="M4" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="32">
+      <c r="M4" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P4" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q4" s="31" t="s">
-        <v>26</v>
-      </c>
+      <c r="P4" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q4" s="28"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="6"/>
-      <c r="B5" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="13" t="s">
-        <v>30</v>
+      <c r="B5" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="8">
+        <v>68</v>
+      </c>
+      <c r="L5" s="42">
         <v>40620</v>
       </c>
-      <c r="M5" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="26">
+      <c r="M5" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P5" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>26</v>
-      </c>
+      <c r="P5" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q5" s="15"/>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="6"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="13" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" s="42">
+        <v>40620</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L6" s="8">
-        <v>40620</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="O6" s="26">
+      <c r="O6" s="24">
         <v>1</v>
       </c>
-      <c r="P6" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>32</v>
-      </c>
+      <c r="P6" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q6" s="15"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="6"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="13" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="13" t="s">
-        <v>38</v>
-      </c>
       <c r="J7" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L7" s="8">
+        <v>103</v>
+      </c>
+      <c r="L7" s="42">
         <v>40620</v>
       </c>
-      <c r="M7" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="O7" s="26">
+      <c r="M7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" s="24">
         <v>1</v>
       </c>
-      <c r="P7" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>32</v>
-      </c>
+      <c r="P7" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q7" s="15"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="6"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="13" t="s">
-        <v>64</v>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="L8" s="8">
+        <v>68</v>
+      </c>
+      <c r="L8" s="42">
         <v>40620</v>
       </c>
-      <c r="M8" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="O8" s="26">
+      <c r="M8" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="O8" s="24">
         <v>1</v>
       </c>
-      <c r="P8" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>32</v>
-      </c>
+      <c r="P8" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q8" s="15"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="6"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="E9" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="L9" s="21">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="E9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="L9" s="44">
         <v>40620</v>
       </c>
-      <c r="M9" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="N9" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="O9" s="27">
+      <c r="M9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="O9" s="25">
         <v>1</v>
       </c>
-      <c r="P9" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q9" s="22" t="s">
-        <v>32</v>
-      </c>
+      <c r="P9" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q9" s="20"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="6"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="13" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="L10" s="42">
+        <v>40620</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L10" s="8">
-        <v>40620</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="O10" s="26">
+      <c r="O10" s="24">
         <v>1</v>
       </c>
-      <c r="P10" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>32</v>
-      </c>
+      <c r="P10" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q10" s="15"/>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="6"/>
-      <c r="B11" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="13" t="s">
+      <c r="B11" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L11" s="42">
+        <v>40620</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="L11" s="8">
-        <v>40620</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="N11" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="O11" s="26">
+      <c r="O11" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P11" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q11" s="16" t="s">
-        <v>32</v>
-      </c>
+      <c r="P11" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q11" s="15"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="6"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="13" t="s">
-        <v>68</v>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="L12" s="8">
+        <v>104</v>
+      </c>
+      <c r="L12" s="42">
         <v>40620</v>
       </c>
-      <c r="M12" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="N12" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="O12" s="26">
+      <c r="M12" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O12" s="24">
         <v>1</v>
       </c>
-      <c r="P12" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q12" s="16" t="s">
-        <v>32</v>
-      </c>
+      <c r="P12" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q12" s="15"/>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="D13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="7" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="L13" s="8">
+        <v>116</v>
+      </c>
+      <c r="L13" s="42">
         <v>40621</v>
       </c>
-      <c r="M13" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="O13" s="26">
+      <c r="M13" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O13" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P13" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q13" s="16" t="s">
-        <v>95</v>
-      </c>
+      <c r="P13" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q13" s="15"/>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="7" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="L14" s="8">
+        <v>79</v>
+      </c>
+      <c r="L14" s="42">
         <v>40622</v>
       </c>
-      <c r="M14" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="N14" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="O14" s="26">
+      <c r="M14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="O14" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P14" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q14" s="16" t="s">
-        <v>96</v>
-      </c>
+      <c r="P14" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q14" s="15"/>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="K15" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="L15" s="21">
+      <c r="E15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="44">
         <v>40623</v>
       </c>
-      <c r="M15" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="N15" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="O15" s="27">
+      <c r="M15" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="O15" s="25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P15" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q15" s="22"/>
+      <c r="P15" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q15" s="20"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="10"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="K16" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="L16" s="21">
+      <c r="I16" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="L16" s="44">
         <v>40623</v>
       </c>
-      <c r="M16" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="N16" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="O16" s="27">
+      <c r="M16" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="O16" s="25">
         <v>1.2</v>
       </c>
-      <c r="P16" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q16" s="22"/>
+      <c r="P16" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q16" s="20"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="K17" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="L17" s="21">
-        <v>40625</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="N17" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="O17" s="27">
-        <v>1.2</v>
-      </c>
-      <c r="P17" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q17" s="22"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="L17" s="42">
+        <v>40624</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="O17" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P17" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q17" s="8"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="L18" s="8">
-        <v>40626</v>
-      </c>
-      <c r="M18" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="N18" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="O18" s="26">
-        <v>1.6</v>
-      </c>
-      <c r="P18" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q18" s="9"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="L18" s="44">
+        <v>40625</v>
+      </c>
+      <c r="M18" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="N18" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="O18" s="25">
+        <v>1.2</v>
+      </c>
+      <c r="P18" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q18" s="20"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="J19" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="K19" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="L19" s="8">
-        <v>40625</v>
-      </c>
-      <c r="M19" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="N19" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="O19" s="26">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P19" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q19" s="9"/>
+      <c r="I19" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="L19" s="44">
+        <v>40626</v>
+      </c>
+      <c r="M19" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="N19" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="O19" s="25">
+        <v>1.6</v>
+      </c>
+      <c r="P19" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q19" s="20"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="14"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="K20" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="L20" s="8">
-        <v>40626</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="N20" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="O20" s="26">
+      <c r="I20" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="L20" s="42">
+        <v>40625</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="N20" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P20" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q20" s="9"/>
+      <c r="P20" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q20" s="8"/>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="10"/>
+      <c r="E21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="13"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="K21" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="L21" s="8">
-        <v>40630</v>
-      </c>
-      <c r="M21" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="N21" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="O21" s="26">
-        <v>1</v>
-      </c>
-      <c r="P21" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q21" s="9"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="L21" s="42">
+        <v>40626</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="O21" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q21" s="8"/>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="J22" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="K22" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L22" s="8">
-        <v>40629</v>
-      </c>
-      <c r="M22" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="N22" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="O22" s="26">
-        <v>1.3</v>
-      </c>
-      <c r="P22" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q22" s="9"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="L22" s="42">
+        <v>40630</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N22" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="O22" s="24">
+        <v>1</v>
+      </c>
+      <c r="P22" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q22" s="8"/>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="J23" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="L23" s="8">
-        <v>40626</v>
-      </c>
-      <c r="M23" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="N23" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="O23" s="26">
-        <v>1.2</v>
-      </c>
-      <c r="P23" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q23" s="9"/>
-    </row>
-    <row r="24" spans="1:17" ht="30">
+      <c r="D23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" s="42">
+        <v>40629</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="O23" s="24">
+        <v>1.3</v>
+      </c>
+      <c r="P23" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q23" s="8"/>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="J24" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="K24" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="L24" s="8">
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="K24" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="42">
         <v>40626</v>
       </c>
-      <c r="M24" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="N24" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="O24" s="26">
-        <v>1</v>
-      </c>
-      <c r="P24" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q24" s="9"/>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="M24" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N24" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O24" s="24">
+        <v>1.2</v>
+      </c>
+      <c r="P24" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="1:17" ht="30">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="29" t="s">
+      <c r="E25" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="K25" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="L25" s="42">
+        <v>40626</v>
+      </c>
+      <c r="M25" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="J25" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K25" s="29" t="s">
+      <c r="N25" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="O25" s="24">
         <v>1</v>
       </c>
-      <c r="L25" s="8">
-        <v>40626</v>
-      </c>
-      <c r="M25" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="N25" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="O25" s="26">
-        <v>1</v>
-      </c>
-      <c r="P25" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q25" s="9"/>
+      <c r="P25" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q25" s="8"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L26" s="8">
-        <v>40630</v>
-      </c>
-      <c r="M26" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="N26" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="O26" s="26">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="K26" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="42">
+        <v>40626</v>
+      </c>
+      <c r="M26" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N26" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="P26" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q26" s="9"/>
+      <c r="O26" s="24">
+        <v>1</v>
+      </c>
+      <c r="P26" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q26" s="8"/>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="29" t="s">
-        <v>142</v>
+      <c r="E27" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="27" t="s">
+        <v>119</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="L27" s="8">
+        <v>96</v>
+      </c>
+      <c r="L27" s="42">
         <v>40630</v>
       </c>
-      <c r="M27" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="N27" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="O27" s="26">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P27" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q27" s="9"/>
+      <c r="M27" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N27" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="O27" s="24">
+        <v>1</v>
+      </c>
+      <c r="P27" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q27" s="8"/>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="7" t="s">
-        <v>150</v>
+      <c r="I28" s="27" t="s">
+        <v>123</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="L28" s="8">
-        <v>40629</v>
-      </c>
-      <c r="M28" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="N28" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="O28" s="26">
-        <v>1.4</v>
-      </c>
-      <c r="P28" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q28" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="L28" s="42">
+        <v>40630</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="N28" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="O28" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P28" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q28" s="8"/>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="6"/>
+      <c r="E29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="33"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="7" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L29" s="8">
-        <v>40631</v>
-      </c>
-      <c r="M29" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="N29" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="O29" s="26">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P29" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q29" s="9"/>
+        <v>104</v>
+      </c>
+      <c r="L29" s="42">
+        <v>40629</v>
+      </c>
+      <c r="M29" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N29" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="O29" s="24">
+        <v>1.4</v>
+      </c>
+      <c r="P29" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q29" s="8"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E30" s="13"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="7" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="K30" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="L30" s="42">
+        <v>40631</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N30" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="O30" s="24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P30" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="L30" s="8">
-        <v>40631</v>
-      </c>
-      <c r="M30" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="N30" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="O30" s="26">
-        <v>1</v>
-      </c>
-      <c r="P30" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q30" s="9"/>
+      <c r="Q30" s="8"/>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L31" s="42">
+        <v>40631</v>
+      </c>
+      <c r="M31" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N31" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="O31" s="24">
+        <v>1</v>
+      </c>
+      <c r="P31" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q31" s="8"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="D32" s="6"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="L32" s="42">
+        <v>40632</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="N32" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="O32" s="24">
+        <v>1</v>
+      </c>
+      <c r="P32" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q32" s="8"/>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
+      <c r="D33" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="E33" s="6"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="L33" s="42">
+        <v>40632</v>
+      </c>
+      <c r="M33" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="N33" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="O33" s="24">
+        <v>1.7</v>
+      </c>
+      <c r="P33" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q33" s="8"/>
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="42"/>
-      <c r="G34" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L34" s="42">
+        <v>40632</v>
+      </c>
+      <c r="M34" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="N34" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="O34" s="24">
+        <v>1</v>
+      </c>
+      <c r="P34" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q34" s="8"/>
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
+      <c r="E35" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="36"/>
+      <c r="G35" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="10"/>
+      <c r="I35" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L35" s="42">
+        <v>40632</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N35" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="O35" s="24">
+        <v>1</v>
+      </c>
+      <c r="P35" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q35" s="8"/>
     </row>
     <row r="36" spans="1:17">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="26"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="L36" s="42">
+        <v>40632</v>
+      </c>
+      <c r="M36" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N36" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="O36" s="24">
+        <v>1</v>
+      </c>
+      <c r="P36" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q36" s="8"/>
     </row>
     <row r="37" spans="1:17">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
+      <c r="E37" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F37" s="13"/>
+      <c r="G37" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="K37" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="L37" s="42">
+        <v>40632</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N37" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="O37" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="P37" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q37" s="8"/>
     </row>
     <row r="38" spans="1:17">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="41"/>
-      <c r="G38" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="L38" s="42">
+        <v>40632</v>
+      </c>
+      <c r="M38" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N38" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="O38" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="P38" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q38" s="8"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
-      <c r="G39" s="15"/>
+      <c r="E39" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="35"/>
+      <c r="G39" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="H39" s="10"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="26"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="45"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
     </row>
     <row r="40" spans="1:17">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F40" s="41"/>
       <c r="G40" s="14"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
     </row>
     <row r="41" spans="1:17">
       <c r="D41" s="6"/>
+      <c r="E41" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="35"/>
+      <c r="G41" s="13"/>
     </row>
     <row r="42" spans="1:17">
       <c r="D42" s="6"/>
-      <c r="E42" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="F42" s="41"/>
-    </row>
-    <row r="44" spans="1:17">
-      <c r="E44" s="16" t="s">
-        <v>148</v>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="D43" s="6"/>
+      <c r="E43" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F43" s="35"/>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="E45" s="15" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3270,8 +3479,9 @@
     <hyperlink ref="P2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>